<commit_message>
[results for traffic data, more results]
</commit_message>
<xml_diff>
--- a/results/results_v2.xlsb.xlsx
+++ b/results/results_v2.xlsb.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TM\Dropbox\DS\RNN-for-TS\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCC7E4F5-4314-4CD0-A7DE-3FFD2A5F9F95}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FDA4C15-D909-486E-955B-56463A92ABAB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="810" windowWidth="19200" windowHeight="7860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10090" yWindow="1560" windowWidth="19200" windowHeight="7860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="37">
   <si>
     <t>Algorithm</t>
   </si>
@@ -503,11 +503,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P62"/>
+  <dimension ref="A1:P65"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A62" sqref="A62"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H44" sqref="H44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -885,35 +885,38 @@
         <v>41.742642977790702</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
+    <row r="14" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E14">
+      <c r="D14" s="7"/>
+      <c r="E14" s="6">
         <v>25</v>
       </c>
-      <c r="F14">
-        <v>1E-3</v>
-      </c>
-      <c r="G14" s="1">
-        <v>50</v>
-      </c>
-      <c r="I14" s="1" t="s">
+      <c r="F14" s="6">
+        <v>1E-3</v>
+      </c>
+      <c r="G14" s="7">
+        <v>50</v>
+      </c>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="K14" s="1">
+      <c r="J14" s="7"/>
+      <c r="K14" s="7">
         <v>3.91654659977242</v>
       </c>
-      <c r="L14">
+      <c r="L14" s="6">
         <v>8.2863294567558601E-2</v>
       </c>
-      <c r="M14">
+      <c r="M14" s="6">
         <v>40.8570696912887</v>
       </c>
-      <c r="P14" s="1" t="s">
+      <c r="P14" s="7" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1519,6 +1522,16 @@
         <v>29</v>
       </c>
     </row>
+    <row r="35" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="C35" s="11"/>
+      <c r="D35" s="11"/>
+      <c r="G35" s="11"/>
+      <c r="H35" s="11"/>
+      <c r="I35" s="11"/>
+      <c r="J35" s="11"/>
+      <c r="K35" s="11"/>
+      <c r="P35" s="11"/>
+    </row>
     <row r="36" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A36" s="2" t="s">
         <v>20</v>
@@ -1714,13 +1727,10 @@
         <v>4227</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E43">
-        <v>100</v>
-      </c>
-      <c r="F43">
-        <v>1E-3</v>
+        <v>25</v>
       </c>
       <c r="G43" s="1">
         <v>50</v>
@@ -1729,19 +1739,19 @@
         <v>42</v>
       </c>
       <c r="K43" s="1">
-        <v>39.8111117321926</v>
-      </c>
-      <c r="L43">
-        <v>0.295085285407581</v>
+        <v>3.7265029427634002</v>
+      </c>
+      <c r="L43" s="1">
+        <v>3.43615135073616E-2</v>
       </c>
       <c r="M43">
-        <v>1532.6129417120101</v>
-      </c>
-      <c r="N43">
-        <v>0.305712224216657</v>
-      </c>
-      <c r="O43">
-        <v>0.28655775903000102</v>
+        <v>45.614512805679603</v>
+      </c>
+      <c r="N43" s="1">
+        <v>3.1547316617100397E-2</v>
+      </c>
+      <c r="O43" s="1">
+        <v>1.5534556490396E-2</v>
       </c>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.35">
@@ -1752,101 +1762,97 @@
         <v>4227</v>
       </c>
       <c r="C44" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E44">
+        <v>25</v>
+      </c>
+      <c r="G44" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>20</v>
+      </c>
+      <c r="B46">
+        <v>4227</v>
+      </c>
+      <c r="C46" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E44">
-        <v>100</v>
-      </c>
-      <c r="F44">
-        <v>1E-3</v>
-      </c>
-      <c r="G44" s="1">
-        <v>100</v>
-      </c>
-      <c r="J44" s="1">
-        <v>42</v>
-      </c>
-      <c r="K44" s="1">
+      <c r="E46">
+        <v>100</v>
+      </c>
+      <c r="F46">
+        <v>1E-3</v>
+      </c>
+      <c r="G46" s="1">
+        <v>50</v>
+      </c>
+      <c r="J46" s="1">
+        <v>42</v>
+      </c>
+      <c r="K46" s="1">
+        <v>39.8111117321926</v>
+      </c>
+      <c r="L46">
+        <v>0.295085285407581</v>
+      </c>
+      <c r="M46">
+        <v>1532.6129417120101</v>
+      </c>
+      <c r="N46">
+        <v>0.305712224216657</v>
+      </c>
+      <c r="O46">
+        <v>0.28655775903000102</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>20</v>
+      </c>
+      <c r="B47">
+        <v>4227</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E47">
+        <v>100</v>
+      </c>
+      <c r="F47">
+        <v>1E-3</v>
+      </c>
+      <c r="G47" s="1">
+        <v>100</v>
+      </c>
+      <c r="J47" s="1">
+        <v>42</v>
+      </c>
+      <c r="K47" s="1">
         <v>24.7464336651162</v>
       </c>
-      <c r="L44" s="1">
+      <c r="L47" s="1">
         <v>0.19131980000000001</v>
       </c>
-      <c r="M44">
+      <c r="M47">
         <v>881.43752107056503</v>
       </c>
-      <c r="N44" s="1">
+      <c r="N47" s="1">
         <v>0.19190260000000001</v>
       </c>
-    </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A45" t="s">
-        <v>20</v>
-      </c>
-      <c r="B45">
-        <v>4227</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E45">
-        <v>100</v>
-      </c>
-      <c r="F45">
-        <v>1E-3</v>
-      </c>
-      <c r="G45" s="1">
-        <v>200</v>
-      </c>
-      <c r="J45" s="1">
-        <v>42</v>
-      </c>
-      <c r="K45" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="L45" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="M45" t="s">
-        <v>28</v>
-      </c>
-      <c r="N45" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="O45" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="P45" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="L46" s="1"/>
-      <c r="N46" s="1"/>
-      <c r="O46" s="1"/>
-    </row>
-    <row r="47" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C47" s="11"/>
-      <c r="D47" s="11"/>
-      <c r="G47" s="11"/>
-      <c r="H47" s="11"/>
-      <c r="I47" s="11"/>
-      <c r="J47" s="11"/>
-      <c r="K47" s="11"/>
-      <c r="P47" s="11"/>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B48">
-        <v>48000</v>
+        <v>4227</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D48" s="1">
-        <v>13463</v>
+        <v>8</v>
       </c>
       <c r="E48">
         <v>100</v>
@@ -1855,105 +1861,44 @@
         <v>1E-3</v>
       </c>
       <c r="G48" s="1">
-        <v>50</v>
+        <v>200</v>
       </c>
       <c r="J48" s="1">
         <v>42</v>
       </c>
-      <c r="K48" s="1">
-        <v>1.2680859933141799</v>
-      </c>
-      <c r="L48">
-        <v>0.14616421362543899</v>
-      </c>
-      <c r="M48">
-        <v>28.511903687299199</v>
-      </c>
-      <c r="N48">
-        <v>0.13301715525572499</v>
+      <c r="K48" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L48" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="M48" t="s">
+        <v>28</v>
+      </c>
+      <c r="N48" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O48" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="P48" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A49" t="s">
-        <v>25</v>
-      </c>
-      <c r="B49">
-        <v>48000</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D49" s="1">
-        <v>13463</v>
-      </c>
-      <c r="E49">
-        <v>100</v>
-      </c>
-      <c r="F49">
-        <v>1E-3</v>
-      </c>
-      <c r="G49" s="1">
-        <v>100</v>
-      </c>
-      <c r="J49" s="1">
-        <v>42</v>
-      </c>
-      <c r="K49" s="1">
-        <v>1.12318553010888</v>
-      </c>
-      <c r="L49">
-        <v>0.14024808260219801</v>
-      </c>
-      <c r="M49">
-        <v>21.9494725945708</v>
-      </c>
-      <c r="N49">
-        <v>0.12659003502329899</v>
-      </c>
-      <c r="O49">
-        <v>8.7821689185904397E-2</v>
-      </c>
-    </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A50" t="s">
-        <v>25</v>
-      </c>
-      <c r="B50">
-        <v>48000</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D50" s="1">
-        <v>13463</v>
-      </c>
-      <c r="E50">
-        <v>100</v>
-      </c>
-      <c r="F50">
-        <v>1E-3</v>
-      </c>
-      <c r="G50" s="1">
-        <v>200</v>
-      </c>
-      <c r="J50" s="1">
-        <v>42</v>
-      </c>
-      <c r="K50" s="1">
-        <v>0.99719524449035302</v>
-      </c>
-      <c r="L50">
-        <v>0.135560354927377</v>
-      </c>
-      <c r="M50">
-        <v>20.7128063902958</v>
-      </c>
-      <c r="N50">
-        <v>0.121544301356057</v>
-      </c>
-      <c r="O50">
-        <v>9.2526590339239004E-2</v>
-      </c>
+      <c r="L49" s="1"/>
+      <c r="N49" s="1"/>
+      <c r="O49" s="1"/>
+    </row>
+    <row r="50" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="C50" s="11"/>
+      <c r="D50" s="11"/>
+      <c r="G50" s="11"/>
+      <c r="H50" s="11"/>
+      <c r="I50" s="11"/>
+      <c r="J50" s="11"/>
+      <c r="K50" s="11"/>
+      <c r="P50" s="11"/>
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
@@ -1975,25 +1920,22 @@
         <v>1E-3</v>
       </c>
       <c r="G51" s="1">
-        <v>400</v>
+        <v>50</v>
       </c>
       <c r="J51" s="1">
         <v>42</v>
       </c>
       <c r="K51" s="1">
-        <v>1.0867464112812699</v>
+        <v>1.2680859933141799</v>
       </c>
       <c r="L51">
-        <v>0.13983351264476401</v>
+        <v>0.14616421362543899</v>
       </c>
       <c r="M51">
-        <v>18.979743834511499</v>
+        <v>28.511903687299199</v>
       </c>
       <c r="N51">
-        <v>0.124734426884066</v>
-      </c>
-      <c r="O51">
-        <v>8.4780461418146394E-2</v>
+        <v>0.13301715525572499</v>
       </c>
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.35">
@@ -2010,31 +1952,31 @@
         <v>13463</v>
       </c>
       <c r="E52">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="F52">
         <v>1E-3</v>
       </c>
       <c r="G52" s="1">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="J52" s="1">
         <v>42</v>
       </c>
       <c r="K52" s="1">
-        <v>1.05958695110418</v>
+        <v>1.12318553010888</v>
       </c>
       <c r="L52">
-        <v>0.137825652728641</v>
+        <v>0.14024808260219801</v>
       </c>
       <c r="M52">
-        <v>20.122850769566899</v>
+        <v>21.9494725945708</v>
       </c>
       <c r="N52">
-        <v>0.123928959665505</v>
+        <v>0.12659003502329899</v>
       </c>
       <c r="O52">
-        <v>8.7829006351591493E-2</v>
+        <v>8.7821689185904397E-2</v>
       </c>
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.35">
@@ -2051,31 +1993,31 @@
         <v>13463</v>
       </c>
       <c r="E53">
+        <v>100</v>
+      </c>
+      <c r="F53">
+        <v>1E-3</v>
+      </c>
+      <c r="G53" s="1">
         <v>200</v>
       </c>
-      <c r="F53">
-        <v>1E-3</v>
-      </c>
-      <c r="G53" s="1">
-        <v>100</v>
-      </c>
       <c r="J53" s="1">
         <v>42</v>
       </c>
       <c r="K53" s="1">
-        <v>1.02581849327672</v>
+        <v>0.99719524449035302</v>
       </c>
       <c r="L53">
-        <v>0.13621914771003299</v>
+        <v>0.135560354927377</v>
       </c>
       <c r="M53">
-        <v>20.7500287533347</v>
+        <v>20.7128063902958</v>
       </c>
       <c r="N53">
-        <v>0.12232933356511901</v>
+        <v>0.121544301356057</v>
       </c>
       <c r="O53">
-        <v>9.2456969482916096E-2</v>
+        <v>9.2526590339239004E-2</v>
       </c>
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.35">
@@ -2092,31 +2034,31 @@
         <v>13463</v>
       </c>
       <c r="E54">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="F54">
         <v>1E-3</v>
       </c>
       <c r="G54" s="1">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="J54" s="1">
         <v>42</v>
       </c>
       <c r="K54" s="1">
-        <v>1.0142830748179701</v>
+        <v>1.0867464112812699</v>
       </c>
       <c r="L54">
-        <v>0.136906633769529</v>
+        <v>0.13983351264476401</v>
       </c>
       <c r="M54">
-        <v>16.218035257216101</v>
+        <v>18.979743834511499</v>
       </c>
       <c r="N54">
-        <v>0.122288426862787</v>
+        <v>0.124734426884066</v>
       </c>
       <c r="O54">
-        <v>8.1100927705568704E-2</v>
+        <v>8.4780461418146394E-2</v>
       </c>
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.35">
@@ -2139,28 +2081,66 @@
         <v>1E-3</v>
       </c>
       <c r="G55" s="1">
-        <v>400</v>
+        <v>50</v>
       </c>
       <c r="J55" s="1">
         <v>42</v>
       </c>
-      <c r="K55" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="L55" t="s">
-        <v>28</v>
-      </c>
-      <c r="M55" t="s">
-        <v>28</v>
-      </c>
-      <c r="N55" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="O55" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="P55" s="1" t="s">
-        <v>35</v>
+      <c r="K55" s="1">
+        <v>1.05958695110418</v>
+      </c>
+      <c r="L55">
+        <v>0.137825652728641</v>
+      </c>
+      <c r="M55">
+        <v>20.122850769566899</v>
+      </c>
+      <c r="N55">
+        <v>0.123928959665505</v>
+      </c>
+      <c r="O55">
+        <v>8.7829006351591493E-2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
+        <v>25</v>
+      </c>
+      <c r="B56">
+        <v>48000</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D56" s="1">
+        <v>13463</v>
+      </c>
+      <c r="E56">
+        <v>200</v>
+      </c>
+      <c r="F56">
+        <v>1E-3</v>
+      </c>
+      <c r="G56" s="1">
+        <v>100</v>
+      </c>
+      <c r="J56" s="1">
+        <v>42</v>
+      </c>
+      <c r="K56" s="1">
+        <v>1.02581849327672</v>
+      </c>
+      <c r="L56">
+        <v>0.13621914771003299</v>
+      </c>
+      <c r="M56">
+        <v>20.7500287533347</v>
+      </c>
+      <c r="N56">
+        <v>0.12232933356511901</v>
+      </c>
+      <c r="O56">
+        <v>9.2456969482916096E-2</v>
       </c>
     </row>
     <row r="57" spans="1:16" x14ac:dyDescent="0.35">
@@ -2171,40 +2151,37 @@
         <v>48000</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D57" s="1">
-        <v>491056</v>
+        <v>13463</v>
       </c>
       <c r="E57">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="F57">
         <v>1E-3</v>
       </c>
       <c r="G57" s="1">
-        <v>50</v>
-      </c>
-      <c r="H57" s="1" t="s">
-        <v>32</v>
+        <v>200</v>
       </c>
       <c r="J57" s="1">
         <v>42</v>
       </c>
       <c r="K57" s="1">
-        <v>119.488322681421</v>
-      </c>
-      <c r="L57" s="1">
-        <v>1.4252456851917701</v>
+        <v>1.0142830748179701</v>
+      </c>
+      <c r="L57">
+        <v>0.136906633769529</v>
       </c>
       <c r="M57">
-        <v>4772.3886078023397</v>
+        <v>16.218035257216101</v>
       </c>
       <c r="N57">
-        <v>11.2135887871412</v>
-      </c>
-      <c r="O57" s="1">
-        <v>3.0093397413643199</v>
+        <v>0.122288426862787</v>
+      </c>
+      <c r="O57">
+        <v>8.1100927705568704E-2</v>
       </c>
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.35">
@@ -2215,88 +2192,176 @@
         <v>48000</v>
       </c>
       <c r="C58" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D58" s="1">
+        <v>13463</v>
+      </c>
+      <c r="E58">
+        <v>200</v>
+      </c>
+      <c r="F58">
+        <v>1E-3</v>
+      </c>
+      <c r="G58" s="1">
+        <v>400</v>
+      </c>
+      <c r="J58" s="1">
+        <v>42</v>
+      </c>
+      <c r="K58" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L58" t="s">
+        <v>28</v>
+      </c>
+      <c r="M58" t="s">
+        <v>28</v>
+      </c>
+      <c r="N58" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O58" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="P58" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="60" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
+        <v>25</v>
+      </c>
+      <c r="B60">
+        <v>48000</v>
+      </c>
+      <c r="C60" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D58" s="1">
+      <c r="D60" s="1">
         <v>491056</v>
       </c>
-      <c r="E58">
-        <v>100</v>
-      </c>
-      <c r="F58">
-        <v>1E-3</v>
-      </c>
-      <c r="G58" s="1">
-        <v>100</v>
-      </c>
-      <c r="J58" s="1">
-        <v>42</v>
-      </c>
-      <c r="K58" s="1">
+      <c r="E60">
+        <v>100</v>
+      </c>
+      <c r="F60">
+        <v>1E-3</v>
+      </c>
+      <c r="G60" s="1">
+        <v>50</v>
+      </c>
+      <c r="H60" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J60" s="1">
+        <v>42</v>
+      </c>
+      <c r="K60" s="1">
+        <v>119.488322681421</v>
+      </c>
+      <c r="L60" s="1">
+        <v>1.4252456851917701</v>
+      </c>
+      <c r="M60">
+        <v>4772.3886078023397</v>
+      </c>
+      <c r="N60">
+        <v>11.2135887871412</v>
+      </c>
+      <c r="O60" s="1">
+        <v>3.0093397413643199</v>
+      </c>
+    </row>
+    <row r="61" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
+        <v>25</v>
+      </c>
+      <c r="B61">
+        <v>48000</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D61" s="1">
+        <v>491056</v>
+      </c>
+      <c r="E61">
+        <v>100</v>
+      </c>
+      <c r="F61">
+        <v>1E-3</v>
+      </c>
+      <c r="G61" s="1">
+        <v>100</v>
+      </c>
+      <c r="J61" s="1">
+        <v>42</v>
+      </c>
+      <c r="K61" s="1">
         <v>106.22708353048699</v>
       </c>
-      <c r="L58">
+      <c r="L61">
         <v>1.47356738153907</v>
       </c>
-      <c r="M58">
+      <c r="M61">
         <v>4241.8667773541902</v>
       </c>
-      <c r="N58">
+      <c r="N61">
         <v>9.4582211159614697</v>
       </c>
-      <c r="O58">
+      <c r="O61">
         <v>2.7352949638966999</v>
       </c>
-      <c r="P58" s="1" t="s">
+      <c r="P61" s="1" t="s">
         <v>33</v>
-      </c>
-    </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A59" t="s">
-        <v>25</v>
-      </c>
-      <c r="B59">
-        <v>48000</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D59" s="1">
-        <v>491056</v>
-      </c>
-      <c r="E59">
-        <v>100</v>
-      </c>
-      <c r="F59">
-        <v>1E-3</v>
-      </c>
-      <c r="G59" s="1">
-        <v>150</v>
       </c>
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
+        <v>25</v>
+      </c>
+      <c r="B62">
+        <v>48000</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D62" s="1">
+        <v>491056</v>
+      </c>
+      <c r="E62">
+        <v>100</v>
+      </c>
+      <c r="F62">
+        <v>1E-3</v>
+      </c>
+      <c r="G62" s="1">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A65" t="s">
         <v>36</v>
       </c>
-      <c r="B62">
+      <c r="B65">
         <v>23000</v>
       </c>
-      <c r="C62" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D62" s="1">
+      <c r="C65" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D65" s="1">
         <v>13463</v>
       </c>
-      <c r="E62">
-        <v>100</v>
-      </c>
-      <c r="F62">
-        <v>1E-3</v>
-      </c>
-      <c r="G62" s="1">
-        <v>50</v>
-      </c>
-      <c r="J62" s="1">
+      <c r="E65">
+        <v>100</v>
+      </c>
+      <c r="F65">
+        <v>1E-3</v>
+      </c>
+      <c r="G65" s="1">
+        <v>50</v>
+      </c>
+      <c r="J65" s="1">
         <v>42</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[update nb DeepAR auto and results]
</commit_message>
<xml_diff>
--- a/results/results_v2.xlsb.xlsx
+++ b/results/results_v2.xlsb.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TM\Dropbox\DS\RNN-for-TS\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{233ED495-0ED4-4FD8-B1B3-07C7D5F057B8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6B5669C-57F6-418B-A177-01EAFD19715F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2340" windowWidth="19200" windowHeight="7860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="776" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="870" uniqueCount="173">
   <si>
     <t>Algorithm</t>
   </si>
@@ -429,6 +429,126 @@
   </si>
   <si>
     <t>2.1920 (299)</t>
+  </si>
+  <si>
+    <t>2.2826 (366)</t>
+  </si>
+  <si>
+    <t>2.1495 (283)</t>
+  </si>
+  <si>
+    <t>batches</t>
+  </si>
+  <si>
+    <t>training/ prediction range</t>
+  </si>
+  <si>
+    <t>use feat static</t>
+  </si>
+  <si>
+    <t>Final training loss</t>
+  </si>
+  <si>
+    <t>w50QLoss</t>
+  </si>
+  <si>
+    <t>w90QLoss</t>
+  </si>
+  <si>
+    <t>44254.4273 (94)</t>
+  </si>
+  <si>
+    <t>11242.94591 (99)</t>
+  </si>
+  <si>
+    <t>18048.4417292 (98)</t>
+  </si>
+  <si>
+    <t>26468.6471 (144)</t>
+  </si>
+  <si>
+    <t>3002.1730 (137)</t>
+  </si>
+  <si>
+    <t>2009.2822 (139)</t>
+  </si>
+  <si>
+    <t>22578.8508 (199)</t>
+  </si>
+  <si>
+    <t>2256.8113 (199)</t>
+  </si>
+  <si>
+    <t>30min</t>
+  </si>
+  <si>
+    <t>860.3205 (199)</t>
+  </si>
+  <si>
+    <t>31min</t>
+  </si>
+  <si>
+    <t>20338.1984 (248)</t>
+  </si>
+  <si>
+    <t>38min</t>
+  </si>
+  <si>
+    <t>1824.8130 (248)</t>
+  </si>
+  <si>
+    <t>39min</t>
+  </si>
+  <si>
+    <t>688.4422 (248)</t>
+  </si>
+  <si>
+    <t>1700.186831563 (497)</t>
+  </si>
+  <si>
+    <t>1h16min</t>
+  </si>
+  <si>
+    <t>616.2295 (496)</t>
+  </si>
+  <si>
+    <t>1h17min</t>
+  </si>
+  <si>
+    <t>342.5092 (497)</t>
+  </si>
+  <si>
+    <t>1h14min</t>
+  </si>
+  <si>
+    <t>68324.1068 (88)</t>
+  </si>
+  <si>
+    <t>layers=(2,2)</t>
+  </si>
+  <si>
+    <t>layers</t>
+  </si>
+  <si>
+    <t>27min</t>
+  </si>
+  <si>
+    <t>32959.7792 (136)</t>
+  </si>
+  <si>
+    <t>41min</t>
+  </si>
+  <si>
+    <t>42528.9749 (199)</t>
+  </si>
+  <si>
+    <t>56min</t>
+  </si>
+  <si>
+    <t>27726.3964 (248)</t>
+  </si>
+  <si>
+    <t>4131.0536 (288)</t>
   </si>
 </sst>
 </file>
@@ -519,7 +639,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -652,6 +772,14 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -932,21 +1060,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25E1F683-F06B-4E20-80D1-BE6D024EC21F}">
-  <dimension ref="A1:P40"/>
+  <dimension ref="A1:Q58"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J23" sqref="J23"/>
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A58" sqref="A58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="4.08984375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.36328125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.7265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.36328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.453125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="11.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="10" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" s="10" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
         <v>7</v>
       </c>
@@ -972,31 +1105,34 @@
         <v>40</v>
       </c>
       <c r="I1" s="11" t="s">
+        <v>165</v>
+      </c>
+      <c r="J1" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="J1" s="11" t="s">
+      <c r="K1" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="K1" s="11" t="s">
+      <c r="L1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="L1" s="10" t="s">
+      <c r="M1" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="M1" s="10" t="s">
+      <c r="N1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="N1" s="11" t="s">
+      <c r="O1" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="O1" s="11" t="s">
+      <c r="P1" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="P1" s="11" t="s">
+      <c r="Q1" s="11" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>16</v>
       </c>
@@ -1017,20 +1153,21 @@
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
-      <c r="K2" s="14">
+      <c r="K2" s="3"/>
+      <c r="L2" s="14">
         <v>2.2608650663714398</v>
       </c>
-      <c r="L2" s="15">
+      <c r="M2" s="15">
         <v>28.196347731740801</v>
       </c>
-      <c r="M2" s="15">
+      <c r="N2" s="15">
         <v>0.14185608409783801</v>
       </c>
-      <c r="N2" s="15"/>
       <c r="O2" s="15"/>
-      <c r="P2" s="3"/>
-    </row>
-    <row r="3" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="P2" s="15"/>
+      <c r="Q2" s="3"/>
+    </row>
+    <row r="3" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
       <c r="F3" s="3"/>
@@ -1038,14 +1175,15 @@
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
-      <c r="K3" s="14"/>
-      <c r="L3" s="15"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="14"/>
       <c r="M3" s="15"/>
       <c r="N3" s="15"/>
       <c r="O3" s="15"/>
-      <c r="P3" s="3"/>
-    </row>
-    <row r="4" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="P3" s="15"/>
+      <c r="Q3" s="3"/>
+    </row>
+    <row r="4" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="F4" s="3"/>
@@ -1053,14 +1191,15 @@
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
-      <c r="K4" s="14"/>
-      <c r="L4" s="15"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="14"/>
       <c r="M4" s="15"/>
       <c r="N4" s="15"/>
       <c r="O4" s="15"/>
-      <c r="P4" s="3"/>
-    </row>
-    <row r="5" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="P4" s="15"/>
+      <c r="Q4" s="3"/>
+    </row>
+    <row r="5" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="F5" s="3"/>
@@ -1068,14 +1207,15 @@
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
-      <c r="K5" s="14"/>
-      <c r="L5" s="15"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="14"/>
       <c r="M5" s="15"/>
       <c r="N5" s="15"/>
       <c r="O5" s="15"/>
-      <c r="P5" s="3"/>
-    </row>
-    <row r="6" spans="1:16" s="33" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="P5" s="15"/>
+      <c r="Q5" s="3"/>
+    </row>
+    <row r="6" spans="1:17" s="33" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="33" t="s">
         <v>16</v>
       </c>
@@ -1096,20 +1236,21 @@
       <c r="H6" s="34"/>
       <c r="I6" s="34"/>
       <c r="J6" s="34"/>
-      <c r="K6" s="35">
+      <c r="K6" s="34"/>
+      <c r="L6" s="35">
         <v>1.44666660175531</v>
       </c>
-      <c r="L6" s="36">
+      <c r="M6" s="36">
         <v>16.642986874988399</v>
       </c>
-      <c r="M6" s="36">
+      <c r="N6" s="36">
         <v>0.1298174584541</v>
       </c>
-      <c r="N6" s="36"/>
       <c r="O6" s="36"/>
-      <c r="P6" s="34"/>
-    </row>
-    <row r="7" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="P6" s="36"/>
+      <c r="Q6" s="34"/>
+    </row>
+    <row r="7" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>16</v>
       </c>
@@ -1128,24 +1269,25 @@
       </c>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
-      <c r="I7" s="3">
+      <c r="I7" s="3"/>
+      <c r="J7" s="3">
         <v>42</v>
       </c>
-      <c r="J7" s="3"/>
-      <c r="K7" s="14">
+      <c r="K7" s="3"/>
+      <c r="L7" s="14">
         <v>1.7621786881972099</v>
       </c>
-      <c r="L7" s="15">
+      <c r="M7" s="15">
         <v>24.567364629029498</v>
       </c>
-      <c r="M7" s="15">
+      <c r="N7" s="15">
         <v>0.136582885212886</v>
       </c>
-      <c r="N7" s="15"/>
       <c r="O7" s="15"/>
-      <c r="P7" s="3"/>
-    </row>
-    <row r="8" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="P7" s="15"/>
+      <c r="Q7" s="3"/>
+    </row>
+    <row r="8" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>16</v>
       </c>
@@ -1166,20 +1308,21 @@
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
-      <c r="K8" s="14">
+      <c r="K8" s="3"/>
+      <c r="L8" s="14">
         <v>2.1688713732443401</v>
       </c>
-      <c r="L8" s="15">
+      <c r="M8" s="15">
         <v>30.985507904866601</v>
       </c>
-      <c r="M8" s="15">
+      <c r="N8" s="15">
         <v>0.13595743149248801</v>
       </c>
-      <c r="N8" s="15"/>
       <c r="O8" s="15"/>
-      <c r="P8" s="3"/>
-    </row>
-    <row r="9" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="P8" s="15"/>
+      <c r="Q8" s="3"/>
+    </row>
+    <row r="9" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>16</v>
       </c>
@@ -1200,28 +1343,29 @@
       </c>
       <c r="G9" s="3"/>
       <c r="H9" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
-      <c r="K9" s="14">
+      <c r="K9" s="3"/>
+      <c r="L9" s="14">
         <v>1.3722961783182199</v>
       </c>
-      <c r="L9" s="15">
+      <c r="M9" s="15">
         <v>24.437912268592498</v>
       </c>
-      <c r="M9" s="15">
+      <c r="N9" s="15">
         <v>0.114591133679717</v>
       </c>
-      <c r="N9" s="15">
+      <c r="O9" s="15">
         <v>6.6035595238716396E-2</v>
       </c>
-      <c r="O9" s="15">
+      <c r="P9" s="15">
         <v>2.7685366126353701E-2</v>
       </c>
-      <c r="P9" s="3"/>
-    </row>
-    <row r="10" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="Q9" s="3"/>
+    </row>
+    <row r="10" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>16</v>
       </c>
@@ -1242,30 +1386,31 @@
       </c>
       <c r="G10" s="3"/>
       <c r="H10" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3">
         <v>42</v>
       </c>
-      <c r="I10" s="3">
-        <v>42</v>
-      </c>
-      <c r="J10" s="3"/>
-      <c r="K10" s="14">
+      <c r="K10" s="3"/>
+      <c r="L10" s="14">
         <v>1.33949444468741</v>
       </c>
-      <c r="L10" s="15">
+      <c r="M10" s="15">
         <v>21.7360339597105</v>
       </c>
-      <c r="M10" s="15">
+      <c r="N10" s="15">
         <v>0.113995292100149</v>
       </c>
-      <c r="N10" s="15">
+      <c r="O10" s="15">
         <v>4.8259866736034197E-2</v>
       </c>
-      <c r="O10" s="15">
+      <c r="P10" s="15">
         <v>3.1924357692853303E-2</v>
       </c>
-      <c r="P10" s="3"/>
-    </row>
-    <row r="11" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="Q10" s="3"/>
+    </row>
+    <row r="11" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>16</v>
       </c>
@@ -1286,30 +1431,31 @@
       </c>
       <c r="G11" s="3"/>
       <c r="H11" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="I11" s="3">
+        <v>41</v>
+      </c>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3">
         <v>43</v>
       </c>
-      <c r="J11" s="3"/>
-      <c r="K11" s="14">
+      <c r="K11" s="3"/>
+      <c r="L11" s="14">
         <v>1.4937566658690999</v>
       </c>
-      <c r="L11" s="15">
+      <c r="M11" s="15">
         <v>27.8690670554127</v>
       </c>
-      <c r="M11" s="15">
+      <c r="N11" s="15">
         <v>0.12576014591313101</v>
       </c>
-      <c r="N11" s="14">
+      <c r="O11" s="14">
         <v>6.4116617488500201E-3</v>
       </c>
-      <c r="O11" s="14">
+      <c r="P11" s="14">
         <v>2.4003126083275102E-2</v>
       </c>
-      <c r="P11" s="3"/>
-    </row>
-    <row r="12" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="Q11" s="3"/>
+    </row>
+    <row r="12" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>16</v>
       </c>
@@ -1330,30 +1476,31 @@
       </c>
       <c r="G12" s="3"/>
       <c r="H12" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="I12" s="3">
+        <v>41</v>
+      </c>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3">
         <v>44</v>
       </c>
-      <c r="J12" s="3"/>
-      <c r="K12" s="14">
+      <c r="K12" s="3"/>
+      <c r="L12" s="14">
         <v>2.1626611472158301</v>
       </c>
-      <c r="L12" s="15">
+      <c r="M12" s="15">
         <v>47.482280539307197</v>
       </c>
-      <c r="M12" s="15">
+      <c r="N12" s="15">
         <v>0.142073465022688</v>
       </c>
-      <c r="N12" s="15">
+      <c r="O12" s="15">
         <v>0.13483371537754801</v>
       </c>
-      <c r="O12" s="15">
+      <c r="P12" s="15">
         <v>0.18224809686688601</v>
       </c>
-      <c r="P12" s="3"/>
-    </row>
-    <row r="13" spans="1:16" s="58" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="Q12" s="3"/>
+    </row>
+    <row r="13" spans="1:17" s="58" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A13" s="58" t="s">
         <v>16</v>
       </c>
@@ -1376,30 +1523,31 @@
       <c r="H13" s="59" t="s">
         <v>41</v>
       </c>
-      <c r="I13" s="59">
+      <c r="I13" s="59"/>
+      <c r="J13" s="59">
         <v>42</v>
       </c>
-      <c r="J13" s="59" t="s">
+      <c r="K13" s="59" t="s">
         <v>126</v>
       </c>
-      <c r="K13" s="60">
+      <c r="L13" s="60">
         <v>1.49276655</v>
       </c>
-      <c r="L13" s="61">
+      <c r="M13" s="61">
         <v>30.277210289999999</v>
       </c>
-      <c r="M13" s="61">
+      <c r="N13" s="61">
         <v>0.11322310612</v>
       </c>
-      <c r="N13" s="61">
+      <c r="O13" s="61">
         <v>4.9931821835000001E-2</v>
       </c>
-      <c r="O13" s="61">
+      <c r="P13" s="61">
         <v>3.0418351361999999E-2</v>
       </c>
-      <c r="P13" s="59"/>
-    </row>
-    <row r="14" spans="1:16" s="58" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="Q13" s="59"/>
+    </row>
+    <row r="14" spans="1:17" s="58" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A14" s="58" t="s">
         <v>16</v>
       </c>
@@ -1422,30 +1570,31 @@
       <c r="H14" s="59" t="s">
         <v>41</v>
       </c>
-      <c r="I14" s="59">
+      <c r="I14" s="59"/>
+      <c r="J14" s="59">
         <v>43</v>
       </c>
-      <c r="J14" s="59" t="s">
+      <c r="K14" s="59" t="s">
         <v>127</v>
       </c>
-      <c r="K14" s="60">
+      <c r="L14" s="60">
         <v>1.5034351163749999</v>
       </c>
-      <c r="L14" s="61">
+      <c r="M14" s="61">
         <v>28.908985919999999</v>
       </c>
-      <c r="M14" s="61">
+      <c r="N14" s="61">
         <v>0.12596107578900001</v>
       </c>
-      <c r="N14" s="61">
+      <c r="O14" s="61">
         <v>6.09939158E-2</v>
       </c>
-      <c r="O14" s="61">
+      <c r="P14" s="61">
         <v>2.36980818E-2</v>
       </c>
-      <c r="P14" s="59"/>
-    </row>
-    <row r="15" spans="1:16" s="58" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="Q14" s="59"/>
+    </row>
+    <row r="15" spans="1:17" s="58" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A15" s="58" t="s">
         <v>16</v>
       </c>
@@ -1468,30 +1617,31 @@
       <c r="H15" s="59" t="s">
         <v>41</v>
       </c>
-      <c r="I15" s="59">
+      <c r="I15" s="59"/>
+      <c r="J15" s="59">
         <v>44</v>
       </c>
-      <c r="J15" s="59" t="s">
+      <c r="K15" s="59" t="s">
         <v>128</v>
       </c>
-      <c r="K15" s="60">
+      <c r="L15" s="60">
         <v>1.5602193</v>
       </c>
-      <c r="L15" s="61">
+      <c r="M15" s="61">
         <v>34.269888151810001</v>
       </c>
-      <c r="M15" s="61">
+      <c r="N15" s="61">
         <v>0.13526352999999999</v>
       </c>
-      <c r="N15" s="61">
+      <c r="O15" s="61">
         <v>0.13921045300000001</v>
       </c>
-      <c r="O15" s="61">
+      <c r="P15" s="61">
         <v>0.19799692999999999</v>
       </c>
-      <c r="P15" s="59"/>
-    </row>
-    <row r="16" spans="1:16" s="58" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="Q15" s="59"/>
+    </row>
+    <row r="16" spans="1:17" s="58" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A16" s="58" t="s">
         <v>16</v>
       </c>
@@ -1514,30 +1664,31 @@
       <c r="H16" s="59" t="s">
         <v>41</v>
       </c>
-      <c r="I16" s="59">
+      <c r="I16" s="59"/>
+      <c r="J16" s="59">
         <v>42</v>
       </c>
-      <c r="J16" s="59" t="s">
+      <c r="K16" s="59" t="s">
         <v>129</v>
       </c>
-      <c r="K16" s="60">
+      <c r="L16" s="60">
         <v>1.3969220821999999</v>
       </c>
-      <c r="L16" s="61">
+      <c r="M16" s="61">
         <v>27.981724400000001</v>
       </c>
-      <c r="M16" s="61">
+      <c r="N16" s="61">
         <v>0.111900554927</v>
       </c>
-      <c r="N16" s="61">
+      <c r="O16" s="61">
         <v>5.0207332389999998E-2</v>
       </c>
-      <c r="O16" s="61">
+      <c r="P16" s="61">
         <v>3.0709150000000001E-2</v>
       </c>
-      <c r="P16" s="59"/>
-    </row>
-    <row r="17" spans="1:16" s="58" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="Q16" s="59"/>
+    </row>
+    <row r="17" spans="1:17" s="58" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A17" s="58" t="s">
         <v>16</v>
       </c>
@@ -1560,30 +1711,31 @@
       <c r="H17" s="59" t="s">
         <v>41</v>
       </c>
-      <c r="I17" s="59">
+      <c r="I17" s="59"/>
+      <c r="J17" s="59">
         <v>43</v>
       </c>
-      <c r="J17" s="59" t="s">
+      <c r="K17" s="59" t="s">
         <v>130</v>
       </c>
-      <c r="K17" s="60">
+      <c r="L17" s="60">
         <v>1.4291122602699999</v>
       </c>
-      <c r="L17" s="61">
+      <c r="M17" s="61">
         <v>27.870253036779999</v>
       </c>
-      <c r="M17" s="61">
+      <c r="N17" s="61">
         <v>0.12589958700000001</v>
       </c>
-      <c r="N17" s="61">
+      <c r="O17" s="61">
         <v>7.6945933999999994E-2</v>
       </c>
-      <c r="O17" s="61">
+      <c r="P17" s="61">
         <v>2.5308649999999999E-2</v>
       </c>
-      <c r="P17" s="59"/>
-    </row>
-    <row r="18" spans="1:16" s="58" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="Q17" s="59"/>
+    </row>
+    <row r="18" spans="1:17" s="58" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A18" s="58" t="s">
         <v>16</v>
       </c>
@@ -1606,30 +1758,31 @@
       <c r="H18" s="59" t="s">
         <v>41</v>
       </c>
-      <c r="I18" s="59">
+      <c r="I18" s="59"/>
+      <c r="J18" s="59">
         <v>44</v>
       </c>
-      <c r="J18" s="59" t="s">
+      <c r="K18" s="59" t="s">
         <v>131</v>
       </c>
-      <c r="K18" s="60">
+      <c r="L18" s="60">
         <v>1.5605943</v>
       </c>
-      <c r="L18" s="61">
+      <c r="M18" s="61">
         <v>35.226810027699997</v>
       </c>
-      <c r="M18" s="61">
+      <c r="N18" s="61">
         <v>0.13552497799999999</v>
       </c>
-      <c r="N18" s="61">
+      <c r="O18" s="61">
         <v>0.14334861600000001</v>
       </c>
-      <c r="O18" s="61">
+      <c r="P18" s="61">
         <v>0.20880326099999999</v>
       </c>
-      <c r="P18" s="59"/>
-    </row>
-    <row r="19" spans="1:16" s="58" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="Q18" s="59"/>
+    </row>
+    <row r="19" spans="1:17" s="58" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A19" s="58" t="s">
         <v>16</v>
       </c>
@@ -1652,30 +1805,31 @@
       <c r="H19" s="59" t="s">
         <v>41</v>
       </c>
-      <c r="I19" s="59">
+      <c r="I19" s="59"/>
+      <c r="J19" s="59">
         <v>42</v>
       </c>
-      <c r="J19" s="59" t="s">
+      <c r="K19" s="59" t="s">
         <v>129</v>
       </c>
-      <c r="K19" s="60">
+      <c r="L19" s="60">
         <v>1.3963500959999999</v>
       </c>
-      <c r="L19" s="61">
+      <c r="M19" s="61">
         <v>27.944284639999999</v>
       </c>
-      <c r="M19" s="61">
+      <c r="N19" s="61">
         <v>0.11220346755000001</v>
       </c>
-      <c r="N19" s="61">
+      <c r="O19" s="61">
         <v>5.0293409999999997E-2</v>
       </c>
-      <c r="O19" s="61">
+      <c r="P19" s="61">
         <v>3.07888542192464E-2</v>
       </c>
-      <c r="P19" s="59"/>
-    </row>
-    <row r="20" spans="1:16" s="58" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="Q19" s="59"/>
+    </row>
+    <row r="20" spans="1:17" s="58" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A20" s="58" t="s">
         <v>16</v>
       </c>
@@ -1698,30 +1852,31 @@
       <c r="H20" s="59" t="s">
         <v>41</v>
       </c>
-      <c r="I20" s="59">
+      <c r="I20" s="59"/>
+      <c r="J20" s="59">
         <v>43</v>
       </c>
-      <c r="J20" s="59" t="s">
+      <c r="K20" s="59" t="s">
         <v>130</v>
       </c>
-      <c r="K20" s="60">
+      <c r="L20" s="60">
         <v>1.4277366968</v>
       </c>
-      <c r="L20" s="61">
+      <c r="M20" s="61">
         <v>27.732527999999999</v>
       </c>
-      <c r="M20" s="61">
+      <c r="N20" s="61">
         <v>0.12604470000000001</v>
       </c>
-      <c r="N20" s="61">
+      <c r="O20" s="61">
         <v>7.7052103699999999E-2</v>
       </c>
-      <c r="O20" s="61">
+      <c r="P20" s="61">
         <v>2.5300769588799999E-2</v>
       </c>
-      <c r="P20" s="59"/>
-    </row>
-    <row r="21" spans="1:16" s="58" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="Q20" s="59"/>
+    </row>
+    <row r="21" spans="1:17" s="58" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A21" s="58" t="s">
         <v>16</v>
       </c>
@@ -1744,30 +1899,31 @@
       <c r="H21" s="59" t="s">
         <v>41</v>
       </c>
-      <c r="I21" s="59">
+      <c r="I21" s="59"/>
+      <c r="J21" s="59">
         <v>44</v>
       </c>
-      <c r="J21" s="59" t="s">
+      <c r="K21" s="59" t="s">
         <v>131</v>
       </c>
-      <c r="K21" s="60">
+      <c r="L21" s="60">
         <v>1.56050280405</v>
       </c>
-      <c r="L21" s="61">
+      <c r="M21" s="61">
         <v>35.201096</v>
       </c>
-      <c r="M21" s="61">
+      <c r="N21" s="61">
         <v>0.13568655512800001</v>
       </c>
-      <c r="N21" s="61">
+      <c r="O21" s="61">
         <v>0.143266808</v>
       </c>
-      <c r="O21" s="61">
+      <c r="P21" s="61">
         <v>0.20868989099999999</v>
       </c>
-      <c r="P21" s="59"/>
-    </row>
-    <row r="22" spans="1:16" s="58" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="Q21" s="59"/>
+    </row>
+    <row r="22" spans="1:17" s="58" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A22" s="58" t="s">
         <v>16</v>
       </c>
@@ -1790,30 +1946,31 @@
       <c r="H22" s="59" t="s">
         <v>41</v>
       </c>
-      <c r="I22" s="59">
+      <c r="I22" s="59"/>
+      <c r="J22" s="59">
         <v>42</v>
       </c>
-      <c r="J22" s="59" t="s">
+      <c r="K22" s="59" t="s">
         <v>132</v>
       </c>
-      <c r="K22" s="60">
+      <c r="L22" s="60">
         <v>1.3396147432100001</v>
       </c>
-      <c r="L22" s="61">
+      <c r="M22" s="61">
         <v>26.626775760000001</v>
       </c>
-      <c r="M22" s="61">
+      <c r="N22" s="61">
         <v>0.109289781788</v>
       </c>
-      <c r="N22" s="61">
+      <c r="O22" s="61">
         <v>4.70859E-2</v>
       </c>
-      <c r="O22" s="61">
+      <c r="P22" s="61">
         <v>3.8158069000000003E-2</v>
       </c>
-      <c r="P22" s="59"/>
-    </row>
-    <row r="23" spans="1:16" s="58" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="Q22" s="59"/>
+    </row>
+    <row r="23" spans="1:17" s="58" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A23" s="58" t="s">
         <v>16</v>
       </c>
@@ -1836,18 +1993,31 @@
       <c r="H23" s="59" t="s">
         <v>41</v>
       </c>
-      <c r="I23" s="59">
+      <c r="I23" s="59"/>
+      <c r="J23" s="59">
         <v>43</v>
       </c>
-      <c r="J23" s="59"/>
-      <c r="K23" s="60"/>
-      <c r="L23" s="61"/>
-      <c r="M23" s="61"/>
-      <c r="N23" s="61"/>
-      <c r="O23" s="61"/>
-      <c r="P23" s="59"/>
-    </row>
-    <row r="24" spans="1:16" s="58" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="K23" s="59" t="s">
+        <v>133</v>
+      </c>
+      <c r="L23" s="60">
+        <v>1.49647760312</v>
+      </c>
+      <c r="M23" s="61">
+        <v>31.595236</v>
+      </c>
+      <c r="N23" s="61">
+        <v>0.123154059944571</v>
+      </c>
+      <c r="O23" s="61">
+        <v>7.3616584994262005E-2</v>
+      </c>
+      <c r="P23" s="61">
+        <v>2.53254359900911E-2</v>
+      </c>
+      <c r="Q23" s="59"/>
+    </row>
+    <row r="24" spans="1:17" s="58" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A24" s="58" t="s">
         <v>16</v>
       </c>
@@ -1870,18 +2040,31 @@
       <c r="H24" s="59" t="s">
         <v>41</v>
       </c>
-      <c r="I24" s="59">
+      <c r="I24" s="59"/>
+      <c r="J24" s="59">
         <v>44</v>
       </c>
-      <c r="J24" s="59"/>
-      <c r="K24" s="60"/>
-      <c r="L24" s="61"/>
-      <c r="M24" s="61"/>
-      <c r="N24" s="61"/>
-      <c r="O24" s="61"/>
-      <c r="P24" s="59"/>
-    </row>
-    <row r="25" spans="1:16" s="58" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="K24" s="59" t="s">
+        <v>134</v>
+      </c>
+      <c r="L24" s="60">
+        <v>1.5429747353900001</v>
+      </c>
+      <c r="M24" s="61">
+        <v>35.371482</v>
+      </c>
+      <c r="N24" s="61">
+        <v>0.13219809499999999</v>
+      </c>
+      <c r="O24" s="61">
+        <v>0.14453732799999999</v>
+      </c>
+      <c r="P24" s="61">
+        <v>0.20880617728</v>
+      </c>
+      <c r="Q24" s="59"/>
+    </row>
+    <row r="25" spans="1:17" s="58" customFormat="1" x14ac:dyDescent="0.35">
       <c r="C25" s="59"/>
       <c r="D25" s="59"/>
       <c r="F25" s="59"/>
@@ -1889,65 +2072,99 @@
       <c r="H25" s="59"/>
       <c r="I25" s="59"/>
       <c r="J25" s="59"/>
-      <c r="K25" s="60"/>
-      <c r="L25" s="61"/>
+      <c r="K25" s="59"/>
+      <c r="L25" s="60"/>
       <c r="M25" s="61"/>
       <c r="N25" s="61"/>
       <c r="O25" s="61"/>
-      <c r="P25" s="59"/>
-    </row>
-    <row r="26" spans="1:16" s="58" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C26" s="59"/>
-      <c r="D26" s="59"/>
-      <c r="F26" s="59"/>
-      <c r="G26" s="59"/>
-      <c r="H26" s="59"/>
-      <c r="I26" s="59"/>
-      <c r="J26" s="59"/>
-      <c r="K26" s="60"/>
-      <c r="L26" s="61"/>
-      <c r="M26" s="61"/>
-      <c r="N26" s="61"/>
-      <c r="O26" s="61"/>
-      <c r="P26" s="59"/>
-    </row>
-    <row r="27" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="4" t="s">
+      <c r="P25" s="61"/>
+      <c r="Q25" s="59"/>
+    </row>
+    <row r="26" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B27" s="4">
+      <c r="B26" s="4">
         <v>414</v>
       </c>
-      <c r="C27" s="5" t="s">
+      <c r="C26" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D27" s="5"/>
-      <c r="E27" s="4">
+      <c r="D26" s="5"/>
+      <c r="E26" s="4">
         <v>25</v>
       </c>
-      <c r="F27" s="5">
-        <v>50</v>
-      </c>
-      <c r="G27" s="5"/>
-      <c r="H27" s="5"/>
-      <c r="I27" s="5"/>
-      <c r="J27" s="5"/>
-      <c r="K27" s="18">
+      <c r="F26" s="5">
+        <v>50</v>
+      </c>
+      <c r="G26" s="5"/>
+      <c r="H26" s="5"/>
+      <c r="I26" s="5"/>
+      <c r="J26" s="5"/>
+      <c r="K26" s="5"/>
+      <c r="L26" s="18">
         <v>2.6633550241579802</v>
       </c>
-      <c r="L27" s="19">
+      <c r="M26" s="19">
         <v>44.230100888809901</v>
       </c>
-      <c r="M27" s="19">
+      <c r="N26" s="19">
         <v>0.181608907022653</v>
       </c>
-      <c r="N27" s="19"/>
-      <c r="O27" s="19"/>
-      <c r="P27" s="5" t="s">
+      <c r="O26" s="19"/>
+      <c r="P26" s="19"/>
+      <c r="Q26" s="5" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="1:16" s="37" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="37" t="s">
+        <v>16</v>
+      </c>
+      <c r="B27" s="37">
+        <v>414</v>
+      </c>
+      <c r="C27" s="38" t="s">
+        <v>5</v>
+      </c>
+      <c r="D27" s="38"/>
+      <c r="E27" s="37">
+        <v>25</v>
+      </c>
+      <c r="F27" s="38">
+        <v>50</v>
+      </c>
+      <c r="G27" s="38" t="s">
+        <v>122</v>
+      </c>
+      <c r="H27" s="38" t="s">
+        <v>42</v>
+      </c>
+      <c r="I27" s="38"/>
+      <c r="J27" s="38">
+        <v>42</v>
+      </c>
+      <c r="K27" s="38">
+        <v>-2.1391</v>
+      </c>
+      <c r="L27" s="39">
+        <v>5.2859148600000001</v>
+      </c>
+      <c r="M27" s="40">
+        <v>106.6797</v>
+      </c>
+      <c r="N27" s="40">
+        <v>0.20337326098</v>
+      </c>
+      <c r="O27" s="40">
+        <v>6.7535999999999999E-2</v>
+      </c>
+      <c r="P27" s="40">
+        <v>8.7957999999999995E-2</v>
+      </c>
+      <c r="Q27" s="38"/>
+    </row>
+    <row r="28" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A28" s="37" t="s">
         <v>16</v>
       </c>
@@ -1970,30 +2187,31 @@
       <c r="H28" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="I28" s="38">
-        <v>42</v>
-      </c>
+      <c r="I28" s="38"/>
       <c r="J28" s="38">
-        <v>-2.1391</v>
-      </c>
-      <c r="K28" s="39">
-        <v>5.2859148600000001</v>
-      </c>
-      <c r="L28" s="40">
-        <v>106.6797</v>
+        <v>43</v>
+      </c>
+      <c r="K28" s="38">
+        <v>-2.1585000000000001</v>
+      </c>
+      <c r="L28" s="39">
+        <v>27.793348000000002</v>
       </c>
       <c r="M28" s="40">
-        <v>0.20337326098</v>
+        <v>248.154777525995</v>
       </c>
       <c r="N28" s="40">
-        <v>6.7535999999999999E-2</v>
+        <v>0.48663820000000002</v>
       </c>
       <c r="O28" s="40">
-        <v>8.7957999999999995E-2</v>
-      </c>
-      <c r="P28" s="38"/>
-    </row>
-    <row r="29" spans="1:16" s="37" customFormat="1" x14ac:dyDescent="0.35">
+        <v>9.5855075562849501E-2</v>
+      </c>
+      <c r="P28" s="40">
+        <v>7.9367781726232295E-2</v>
+      </c>
+      <c r="Q28" s="38"/>
+    </row>
+    <row r="29" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A29" s="37" t="s">
         <v>16</v>
       </c>
@@ -2016,30 +2234,31 @@
       <c r="H29" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="I29" s="38">
-        <v>43</v>
-      </c>
+      <c r="I29" s="38"/>
       <c r="J29" s="38">
-        <v>-2.1585000000000001</v>
-      </c>
-      <c r="K29" s="39">
-        <v>27.793348000000002</v>
-      </c>
-      <c r="L29" s="40">
-        <v>248.154777525995</v>
+        <v>44</v>
+      </c>
+      <c r="K29" s="38">
+        <v>-2.1217999999999999</v>
+      </c>
+      <c r="L29" s="39">
+        <v>13.364979999999999</v>
       </c>
       <c r="M29" s="40">
-        <v>0.48663820000000002</v>
+        <v>102.98322875229999</v>
       </c>
       <c r="N29" s="40">
-        <v>9.5855075562849501E-2</v>
+        <v>0.35098499999999999</v>
       </c>
       <c r="O29" s="40">
-        <v>7.9367781726232295E-2</v>
-      </c>
-      <c r="P29" s="38"/>
-    </row>
-    <row r="30" spans="1:16" s="37" customFormat="1" x14ac:dyDescent="0.35">
+        <v>0.183749</v>
+      </c>
+      <c r="P29" s="40">
+        <v>7.4605900000000003E-2</v>
+      </c>
+      <c r="Q29" s="38"/>
+    </row>
+    <row r="30" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A30" s="37" t="s">
         <v>16</v>
       </c>
@@ -2057,35 +2276,36 @@
         <v>50</v>
       </c>
       <c r="G30" s="38" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="H30" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="I30" s="38">
-        <v>44</v>
-      </c>
+      <c r="I30" s="38"/>
       <c r="J30" s="38">
-        <v>-2.1217999999999999</v>
-      </c>
-      <c r="K30" s="39">
-        <v>13.364979999999999</v>
-      </c>
-      <c r="L30" s="40">
-        <v>102.98322875229999</v>
+        <v>42</v>
+      </c>
+      <c r="K30" s="38">
+        <v>-2.0457999999999998</v>
+      </c>
+      <c r="L30" s="39">
+        <v>1.4336720999999999</v>
       </c>
       <c r="M30" s="40">
-        <v>0.35098499999999999</v>
+        <v>21.056016482362999</v>
       </c>
       <c r="N30" s="40">
-        <v>0.183749</v>
+        <v>0.14271562800000001</v>
       </c>
       <c r="O30" s="40">
-        <v>7.4605900000000003E-2</v>
-      </c>
-      <c r="P30" s="38"/>
-    </row>
-    <row r="31" spans="1:16" s="37" customFormat="1" x14ac:dyDescent="0.35">
+        <v>5.4922392845000001E-2</v>
+      </c>
+      <c r="P30" s="40">
+        <v>2.1950000000000001E-2</v>
+      </c>
+      <c r="Q30" s="38"/>
+    </row>
+    <row r="31" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A31" s="37" t="s">
         <v>16</v>
       </c>
@@ -2108,30 +2328,31 @@
       <c r="H31" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="I31" s="38">
-        <v>42</v>
-      </c>
+      <c r="I31" s="38"/>
       <c r="J31" s="38">
-        <v>-2.0457999999999998</v>
-      </c>
-      <c r="K31" s="39">
-        <v>1.4336720999999999</v>
-      </c>
-      <c r="L31" s="40">
-        <v>21.056016482362999</v>
+        <v>43</v>
+      </c>
+      <c r="K31" s="38">
+        <v>-2.0164</v>
+      </c>
+      <c r="L31" s="39">
+        <v>1.4966787960000001</v>
       </c>
       <c r="M31" s="40">
-        <v>0.14271562800000001</v>
+        <v>21.597083600000001</v>
       </c>
       <c r="N31" s="40">
-        <v>5.4922392845000001E-2</v>
+        <v>0.15133988396055101</v>
       </c>
       <c r="O31" s="40">
-        <v>2.1950000000000001E-2</v>
-      </c>
-      <c r="P31" s="38"/>
-    </row>
-    <row r="32" spans="1:16" s="37" customFormat="1" x14ac:dyDescent="0.35">
+        <v>5.1074555000000001E-2</v>
+      </c>
+      <c r="P31" s="40">
+        <v>2.2300419577265401E-2</v>
+      </c>
+      <c r="Q31" s="38"/>
+    </row>
+    <row r="32" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A32" s="37" t="s">
         <v>16</v>
       </c>
@@ -2154,76 +2375,47 @@
       <c r="H32" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="I32" s="38">
-        <v>43</v>
-      </c>
+      <c r="I32" s="38"/>
       <c r="J32" s="38">
-        <v>-2.0164</v>
-      </c>
-      <c r="K32" s="39">
-        <v>1.4966787960000001</v>
-      </c>
-      <c r="L32" s="40">
-        <v>21.597083600000001</v>
+        <v>44</v>
+      </c>
+      <c r="K32" s="38">
+        <v>-1.9988999999999999</v>
+      </c>
+      <c r="L32" s="39">
+        <v>1.469979618</v>
       </c>
       <c r="M32" s="40">
-        <v>0.15133988396055101</v>
+        <v>21.918610000000001</v>
       </c>
       <c r="N32" s="40">
-        <v>5.1074555000000001E-2</v>
+        <v>0.1521371966</v>
       </c>
       <c r="O32" s="40">
-        <v>2.2300419577265401E-2</v>
-      </c>
-      <c r="P32" s="38"/>
-    </row>
-    <row r="33" spans="1:16" s="37" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="37" t="s">
-        <v>16</v>
-      </c>
-      <c r="B33" s="37">
-        <v>414</v>
-      </c>
-      <c r="C33" s="38" t="s">
-        <v>5</v>
-      </c>
+        <v>5.9614221382261703E-2</v>
+      </c>
+      <c r="P32" s="40">
+        <v>2.2553602133483699E-2</v>
+      </c>
+      <c r="Q32" s="38"/>
+    </row>
+    <row r="33" spans="1:17" s="37" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="C33" s="38"/>
       <c r="D33" s="38"/>
-      <c r="E33" s="37">
-        <v>25</v>
-      </c>
-      <c r="F33" s="38">
-        <v>50</v>
-      </c>
-      <c r="G33" s="38" t="s">
-        <v>123</v>
-      </c>
-      <c r="H33" s="38" t="s">
-        <v>42</v>
-      </c>
-      <c r="I33" s="38">
-        <v>44</v>
-      </c>
-      <c r="J33" s="38">
-        <v>-1.9988999999999999</v>
-      </c>
-      <c r="K33" s="39">
-        <v>1.469979618</v>
-      </c>
-      <c r="L33" s="40">
-        <v>21.918610000000001</v>
-      </c>
-      <c r="M33" s="40">
-        <v>0.1521371966</v>
-      </c>
-      <c r="N33" s="40">
-        <v>5.9614221382261703E-2</v>
-      </c>
-      <c r="O33" s="40">
-        <v>2.2553602133483699E-2</v>
-      </c>
-      <c r="P33" s="38"/>
-    </row>
-    <row r="34" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="F33" s="38"/>
+      <c r="G33" s="38"/>
+      <c r="H33" s="38"/>
+      <c r="I33" s="38"/>
+      <c r="J33" s="38"/>
+      <c r="K33" s="38"/>
+      <c r="L33" s="39"/>
+      <c r="M33" s="40"/>
+      <c r="N33" s="40"/>
+      <c r="O33" s="40"/>
+      <c r="P33" s="40"/>
+      <c r="Q33" s="38"/>
+    </row>
+    <row r="34" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A34" s="37"/>
       <c r="B34" s="37"/>
       <c r="C34" s="38"/>
@@ -2233,15 +2425,16 @@
       <c r="G34" s="38"/>
       <c r="H34" s="38"/>
       <c r="I34" s="38"/>
-      <c r="J34" s="5"/>
-      <c r="K34" s="18"/>
-      <c r="L34" s="19"/>
+      <c r="J34" s="38"/>
+      <c r="K34" s="5"/>
+      <c r="L34" s="18"/>
       <c r="M34" s="19"/>
       <c r="N34" s="19"/>
       <c r="O34" s="19"/>
-      <c r="P34" s="5"/>
-    </row>
-    <row r="35" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="P34" s="19"/>
+      <c r="Q34" s="5"/>
+    </row>
+    <row r="35" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A35" s="6" t="s">
         <v>16</v>
       </c>
@@ -2256,151 +2449,1008 @@
         <v>100</v>
       </c>
       <c r="F35" s="7">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="G35" s="7"/>
       <c r="H35" s="7"/>
-      <c r="I35" s="7">
+      <c r="I35" s="7"/>
+      <c r="J35" s="7">
         <v>42</v>
       </c>
-      <c r="J35" s="7"/>
-      <c r="K35" s="20">
-        <v>13.752988999999999</v>
-      </c>
-      <c r="L35" s="21">
-        <v>260.71834811000002</v>
+      <c r="K35" s="7"/>
+      <c r="L35" s="20">
+        <v>23.533678978716601</v>
       </c>
       <c r="M35" s="21">
-        <v>0.34606221715618302</v>
+        <v>545.75731609802597</v>
       </c>
       <c r="N35" s="21">
-        <v>0.100243507241533</v>
+        <v>0.42155993227215</v>
       </c>
       <c r="O35" s="21">
-        <v>0.118486994896638</v>
-      </c>
-      <c r="P35" s="7"/>
-    </row>
-    <row r="36" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="6" t="s">
+        <v>0.33439627305276798</v>
+      </c>
+      <c r="P35" s="21">
+        <v>8.1370935121077501E-2</v>
+      </c>
+      <c r="Q35" s="7"/>
+    </row>
+    <row r="36" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="B36" s="6">
+      <c r="B36" s="25">
         <v>414</v>
       </c>
-      <c r="C36" s="7" t="s">
+      <c r="C36" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="D36" s="7"/>
-      <c r="E36" s="6">
-        <v>100</v>
-      </c>
-      <c r="F36" s="7">
-        <v>100</v>
-      </c>
-      <c r="G36" s="7"/>
-      <c r="H36" s="7"/>
-      <c r="I36" s="7">
+      <c r="D36" s="26"/>
+      <c r="E36" s="25">
+        <v>100</v>
+      </c>
+      <c r="F36" s="26">
+        <v>200</v>
+      </c>
+      <c r="G36" s="26"/>
+      <c r="H36" s="26"/>
+      <c r="I36" s="26"/>
+      <c r="J36" s="26">
         <v>42</v>
       </c>
-      <c r="J36" s="7"/>
-      <c r="K36" s="20">
-        <v>23.533678978716601</v>
-      </c>
-      <c r="L36" s="21">
-        <v>545.75731609802597</v>
-      </c>
-      <c r="M36" s="21">
-        <v>0.42155993227215</v>
-      </c>
-      <c r="N36" s="21">
-        <v>0.33439627305276798</v>
-      </c>
-      <c r="O36" s="21">
-        <v>8.1370935121077501E-2</v>
-      </c>
-      <c r="P36" s="7"/>
-    </row>
-    <row r="37" spans="1:16" s="25" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="B37" s="25">
-        <v>414</v>
-      </c>
-      <c r="C37" s="26" t="s">
-        <v>8</v>
-      </c>
+      <c r="K36" s="26"/>
+      <c r="L36" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="M36" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="N36" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="O36" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="P36" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q36" s="26" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" s="25" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="C37" s="26"/>
       <c r="D37" s="26"/>
-      <c r="E37" s="25">
-        <v>100</v>
-      </c>
-      <c r="F37" s="26">
-        <v>200</v>
-      </c>
+      <c r="F37" s="26"/>
       <c r="G37" s="26"/>
       <c r="H37" s="26"/>
-      <c r="I37" s="26">
+      <c r="I37" s="26"/>
+      <c r="J37" s="26"/>
+      <c r="K37" s="26"/>
+      <c r="L37" s="26"/>
+      <c r="O37" s="26"/>
+      <c r="P37" s="26"/>
+      <c r="Q37" s="26"/>
+    </row>
+    <row r="38" spans="1:17" s="67" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="41" t="s">
+        <v>16</v>
+      </c>
+      <c r="B38" s="41">
+        <v>414</v>
+      </c>
+      <c r="C38" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="D38" s="42"/>
+      <c r="E38" s="41">
+        <v>100</v>
+      </c>
+      <c r="F38" s="42">
+        <v>50</v>
+      </c>
+      <c r="G38" s="42"/>
+      <c r="H38" s="42"/>
+      <c r="I38" s="42"/>
+      <c r="J38" s="42">
         <v>42</v>
       </c>
-      <c r="J37" s="26"/>
-      <c r="K37" s="26" t="s">
-        <v>23</v>
-      </c>
-      <c r="L37" s="25" t="s">
-        <v>23</v>
-      </c>
-      <c r="M37" s="25" t="s">
-        <v>23</v>
-      </c>
-      <c r="N37" s="26" t="s">
-        <v>23</v>
-      </c>
-      <c r="O37" s="26" t="s">
-        <v>23</v>
-      </c>
-      <c r="P37" s="26" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="38" spans="1:16" s="25" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C38" s="26"/>
-      <c r="D38" s="26"/>
-      <c r="F38" s="26"/>
-      <c r="G38" s="26"/>
-      <c r="H38" s="26"/>
-      <c r="I38" s="26"/>
-      <c r="J38" s="26"/>
-      <c r="K38" s="26"/>
-      <c r="N38" s="26"/>
-      <c r="O38" s="26"/>
-      <c r="P38" s="26"/>
-    </row>
-    <row r="39" spans="1:16" s="25" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C39" s="26"/>
-      <c r="D39" s="26"/>
-      <c r="F39" s="26"/>
-      <c r="G39" s="26"/>
-      <c r="H39" s="26"/>
-      <c r="I39" s="26"/>
-      <c r="J39" s="26"/>
-      <c r="K39" s="26"/>
-      <c r="N39" s="26"/>
-      <c r="O39" s="26"/>
-      <c r="P39" s="26"/>
-    </row>
-    <row r="40" spans="1:16" s="25" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C40" s="26"/>
-      <c r="D40" s="26"/>
-      <c r="F40" s="26"/>
-      <c r="G40" s="26"/>
-      <c r="H40" s="26"/>
-      <c r="I40" s="26"/>
-      <c r="J40" s="26"/>
-      <c r="K40" s="26"/>
-      <c r="N40" s="26"/>
-      <c r="O40" s="26"/>
-      <c r="P40" s="26"/>
+      <c r="K38" s="66" t="s">
+        <v>141</v>
+      </c>
+      <c r="L38" s="68">
+        <v>13.752989064227201</v>
+      </c>
+      <c r="M38" s="69">
+        <v>260.71834811999997</v>
+      </c>
+      <c r="N38" s="69">
+        <v>0.34606221700000001</v>
+      </c>
+      <c r="O38" s="68">
+        <v>0.100243507241533</v>
+      </c>
+      <c r="P38" s="68">
+        <v>0.1184869948966</v>
+      </c>
+      <c r="Q38" s="66"/>
+    </row>
+    <row r="39" spans="1:17" s="67" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="41" t="s">
+        <v>16</v>
+      </c>
+      <c r="B39" s="41">
+        <v>414</v>
+      </c>
+      <c r="C39" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="D39" s="42"/>
+      <c r="E39" s="41">
+        <v>100</v>
+      </c>
+      <c r="F39" s="42">
+        <v>50</v>
+      </c>
+      <c r="G39" s="42"/>
+      <c r="H39" s="42"/>
+      <c r="I39" s="42"/>
+      <c r="J39" s="42">
+        <v>43</v>
+      </c>
+      <c r="K39" s="66" t="s">
+        <v>142</v>
+      </c>
+      <c r="L39" s="68">
+        <v>13.749186987</v>
+      </c>
+      <c r="M39" s="69">
+        <v>234.73750999999999</v>
+      </c>
+      <c r="N39" s="69">
+        <v>0.34225530786530001</v>
+      </c>
+      <c r="O39" s="68">
+        <v>9.7763042491408506E-2</v>
+      </c>
+      <c r="P39" s="68">
+        <v>0.10846537520000001</v>
+      </c>
+      <c r="Q39" s="66"/>
+    </row>
+    <row r="40" spans="1:17" s="41" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="67" t="s">
+        <v>16</v>
+      </c>
+      <c r="B40" s="67">
+        <v>414</v>
+      </c>
+      <c r="C40" s="66" t="s">
+        <v>8</v>
+      </c>
+      <c r="D40" s="66"/>
+      <c r="E40" s="67">
+        <v>100</v>
+      </c>
+      <c r="F40" s="66">
+        <v>50</v>
+      </c>
+      <c r="G40" s="66"/>
+      <c r="H40" s="66"/>
+      <c r="I40" s="66"/>
+      <c r="J40" s="66">
+        <v>44</v>
+      </c>
+      <c r="K40" s="41" t="s">
+        <v>143</v>
+      </c>
+      <c r="L40" s="44">
+        <v>15.0871902949758</v>
+      </c>
+      <c r="M40" s="44">
+        <v>292.86451212999998</v>
+      </c>
+      <c r="N40" s="44">
+        <v>0.35499995299830001</v>
+      </c>
+      <c r="O40" s="44">
+        <v>0.12719792438081401</v>
+      </c>
+      <c r="P40" s="44">
+        <v>0.11211767573500001</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" s="41" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="41" t="s">
+        <v>16</v>
+      </c>
+      <c r="B41" s="41">
+        <v>414</v>
+      </c>
+      <c r="C41" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="D41" s="42"/>
+      <c r="E41" s="41">
+        <v>150</v>
+      </c>
+      <c r="F41" s="42">
+        <v>50</v>
+      </c>
+      <c r="G41" s="42"/>
+      <c r="H41" s="42"/>
+      <c r="I41" s="42"/>
+      <c r="J41" s="42">
+        <v>42</v>
+      </c>
+      <c r="K41" s="42" t="s">
+        <v>144</v>
+      </c>
+      <c r="L41" s="44">
+        <v>14.7165642423</v>
+      </c>
+      <c r="M41" s="44">
+        <v>293.48100548871997</v>
+      </c>
+      <c r="N41" s="44">
+        <v>0.34832704199999998</v>
+      </c>
+      <c r="O41" s="44">
+        <v>8.7628885399999995E-2</v>
+      </c>
+      <c r="P41" s="44">
+        <v>6.6904239000000004E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" s="41" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="41" t="s">
+        <v>16</v>
+      </c>
+      <c r="B42" s="41">
+        <v>414</v>
+      </c>
+      <c r="C42" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="D42" s="42"/>
+      <c r="E42" s="41">
+        <v>150</v>
+      </c>
+      <c r="F42" s="42">
+        <v>50</v>
+      </c>
+      <c r="G42" s="42"/>
+      <c r="H42" s="42"/>
+      <c r="I42" s="42"/>
+      <c r="J42" s="42">
+        <v>43</v>
+      </c>
+      <c r="K42" s="42" t="s">
+        <v>145</v>
+      </c>
+      <c r="L42" s="44">
+        <v>13.969189800000001</v>
+      </c>
+      <c r="M42" s="44">
+        <v>242.00053260022599</v>
+      </c>
+      <c r="N42" s="44">
+        <v>0.34151055159425298</v>
+      </c>
+      <c r="O42" s="44">
+        <v>0.101280667689</v>
+      </c>
+      <c r="P42" s="44">
+        <v>8.6097344000000006E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" s="41" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="67" t="s">
+        <v>16</v>
+      </c>
+      <c r="B43" s="67">
+        <v>414</v>
+      </c>
+      <c r="C43" s="66" t="s">
+        <v>8</v>
+      </c>
+      <c r="D43" s="66"/>
+      <c r="E43" s="41">
+        <v>150</v>
+      </c>
+      <c r="F43" s="66">
+        <v>50</v>
+      </c>
+      <c r="G43" s="66"/>
+      <c r="H43" s="66"/>
+      <c r="I43" s="66"/>
+      <c r="J43" s="66">
+        <v>44</v>
+      </c>
+      <c r="K43" s="42" t="s">
+        <v>146</v>
+      </c>
+      <c r="L43" s="44">
+        <v>15.0451286</v>
+      </c>
+      <c r="M43" s="44">
+        <v>301.010694</v>
+      </c>
+      <c r="N43" s="44">
+        <v>0.33589392000000001</v>
+      </c>
+      <c r="O43" s="44">
+        <v>8.3964380000000005E-2</v>
+      </c>
+      <c r="P43" s="44">
+        <v>8.55931446113503E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17" s="41" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="41" t="s">
+        <v>16</v>
+      </c>
+      <c r="B44" s="41">
+        <v>414</v>
+      </c>
+      <c r="C44" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="D44" s="42"/>
+      <c r="E44" s="41">
+        <v>200</v>
+      </c>
+      <c r="F44" s="42">
+        <v>50</v>
+      </c>
+      <c r="G44" s="42"/>
+      <c r="H44" s="42"/>
+      <c r="I44" s="42"/>
+      <c r="J44" s="42">
+        <v>42</v>
+      </c>
+      <c r="K44" s="41" t="s">
+        <v>147</v>
+      </c>
+      <c r="L44" s="44">
+        <v>15.1654652676</v>
+      </c>
+      <c r="M44" s="44">
+        <v>305.80285329999998</v>
+      </c>
+      <c r="N44" s="44">
+        <v>0.35056138091400002</v>
+      </c>
+      <c r="O44" s="44">
+        <v>9.8102664315859997E-2</v>
+      </c>
+      <c r="P44" s="44">
+        <v>5.0823350000000003E-2</v>
+      </c>
+      <c r="Q44" s="41" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17" s="41" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="41" t="s">
+        <v>16</v>
+      </c>
+      <c r="B45" s="41">
+        <v>414</v>
+      </c>
+      <c r="C45" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="D45" s="42"/>
+      <c r="E45" s="41">
+        <v>200</v>
+      </c>
+      <c r="F45" s="42">
+        <v>50</v>
+      </c>
+      <c r="G45" s="42"/>
+      <c r="H45" s="42"/>
+      <c r="I45" s="42"/>
+      <c r="J45" s="42">
+        <v>43</v>
+      </c>
+      <c r="K45" s="41" t="s">
+        <v>148</v>
+      </c>
+      <c r="L45" s="44">
+        <v>13.959626846999999</v>
+      </c>
+      <c r="M45" s="44">
+        <v>246.59950749999999</v>
+      </c>
+      <c r="N45" s="44">
+        <v>0.33959842979260302</v>
+      </c>
+      <c r="O45" s="44">
+        <v>9.7938040000000004E-2</v>
+      </c>
+      <c r="P45" s="44">
+        <v>7.7259273000000003E-2</v>
+      </c>
+      <c r="Q45" s="41" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17" s="41" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="67" t="s">
+        <v>16</v>
+      </c>
+      <c r="B46" s="67">
+        <v>414</v>
+      </c>
+      <c r="C46" s="66" t="s">
+        <v>8</v>
+      </c>
+      <c r="D46" s="66"/>
+      <c r="E46" s="41">
+        <v>200</v>
+      </c>
+      <c r="F46" s="66">
+        <v>50</v>
+      </c>
+      <c r="G46" s="66"/>
+      <c r="H46" s="66"/>
+      <c r="I46" s="66"/>
+      <c r="J46" s="66">
+        <v>44</v>
+      </c>
+      <c r="K46" s="41" t="s">
+        <v>150</v>
+      </c>
+      <c r="L46" s="44">
+        <v>15.409713</v>
+      </c>
+      <c r="M46" s="44">
+        <v>315.272921333</v>
+      </c>
+      <c r="N46" s="44">
+        <v>0.34231472699999999</v>
+      </c>
+      <c r="O46" s="44">
+        <v>0.10821991</v>
+      </c>
+      <c r="P46" s="44">
+        <v>5.0431223184539999E-2</v>
+      </c>
+      <c r="Q46" s="41" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17" s="41" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="41" t="s">
+        <v>16</v>
+      </c>
+      <c r="B47" s="41">
+        <v>414</v>
+      </c>
+      <c r="C47" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="D47" s="42"/>
+      <c r="E47" s="41">
+        <v>250</v>
+      </c>
+      <c r="F47" s="42">
+        <v>50</v>
+      </c>
+      <c r="G47" s="42"/>
+      <c r="H47" s="42"/>
+      <c r="I47" s="42"/>
+      <c r="J47" s="42">
+        <v>42</v>
+      </c>
+      <c r="K47" s="41" t="s">
+        <v>152</v>
+      </c>
+      <c r="L47" s="41">
+        <v>15.359679653000001</v>
+      </c>
+      <c r="M47" s="41">
+        <v>312.25125229999998</v>
+      </c>
+      <c r="N47" s="41">
+        <v>0.35152056599999998</v>
+      </c>
+      <c r="O47" s="41">
+        <v>9.2657845000000003E-2</v>
+      </c>
+      <c r="P47" s="41">
+        <v>5.2024486170000002E-2</v>
+      </c>
+      <c r="Q47" s="41" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="48" spans="1:17" s="41" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="41" t="s">
+        <v>16</v>
+      </c>
+      <c r="B48" s="41">
+        <v>414</v>
+      </c>
+      <c r="C48" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="D48" s="42"/>
+      <c r="E48" s="41">
+        <v>250</v>
+      </c>
+      <c r="F48" s="42">
+        <v>50</v>
+      </c>
+      <c r="G48" s="42"/>
+      <c r="H48" s="42"/>
+      <c r="I48" s="42"/>
+      <c r="J48" s="42">
+        <v>43</v>
+      </c>
+      <c r="K48" s="41" t="s">
+        <v>154</v>
+      </c>
+      <c r="L48" s="41">
+        <v>14.0866255</v>
+      </c>
+      <c r="M48" s="41">
+        <v>252.81450193000001</v>
+      </c>
+      <c r="N48" s="41">
+        <v>0.33862513189999999</v>
+      </c>
+      <c r="O48" s="41">
+        <v>0.1089630217</v>
+      </c>
+      <c r="P48" s="41">
+        <v>6.7984618234510005E-2</v>
+      </c>
+      <c r="Q48" s="41" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="49" spans="1:17" s="41" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="67" t="s">
+        <v>16</v>
+      </c>
+      <c r="B49" s="67">
+        <v>414</v>
+      </c>
+      <c r="C49" s="66" t="s">
+        <v>8</v>
+      </c>
+      <c r="D49" s="66"/>
+      <c r="E49" s="41">
+        <v>250</v>
+      </c>
+      <c r="F49" s="66">
+        <v>50</v>
+      </c>
+      <c r="G49" s="66"/>
+      <c r="H49" s="66"/>
+      <c r="I49" s="66"/>
+      <c r="J49" s="66">
+        <v>44</v>
+      </c>
+      <c r="K49" s="41" t="s">
+        <v>156</v>
+      </c>
+      <c r="L49" s="41">
+        <v>15.4568707275</v>
+      </c>
+      <c r="M49" s="41">
+        <v>320.67832979999997</v>
+      </c>
+      <c r="N49" s="41">
+        <v>0.3434173807</v>
+      </c>
+      <c r="O49" s="41">
+        <v>0.109215592778</v>
+      </c>
+      <c r="P49" s="41">
+        <v>5.0618870476E-2</v>
+      </c>
+      <c r="Q49" s="41" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="50" spans="1:17" s="41" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="41" t="s">
+        <v>16</v>
+      </c>
+      <c r="B50" s="41">
+        <v>414</v>
+      </c>
+      <c r="C50" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="D50" s="42"/>
+      <c r="E50" s="41">
+        <v>500</v>
+      </c>
+      <c r="F50" s="42">
+        <v>50</v>
+      </c>
+      <c r="G50" s="42"/>
+      <c r="H50" s="42"/>
+      <c r="I50" s="42"/>
+      <c r="J50" s="42">
+        <v>42</v>
+      </c>
+      <c r="K50" s="41" t="s">
+        <v>157</v>
+      </c>
+      <c r="L50" s="41">
+        <v>16.5050431889875</v>
+      </c>
+      <c r="M50" s="41">
+        <v>352.23572202418899</v>
+      </c>
+      <c r="N50" s="41">
+        <v>0.36345001403593702</v>
+      </c>
+      <c r="O50" s="41">
+        <v>0.149904881236786</v>
+      </c>
+      <c r="P50" s="41">
+        <v>5.1993752166000003E-2</v>
+      </c>
+      <c r="Q50" s="41" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="51" spans="1:17" s="41" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A51" s="41" t="s">
+        <v>16</v>
+      </c>
+      <c r="B51" s="41">
+        <v>414</v>
+      </c>
+      <c r="C51" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="D51" s="42"/>
+      <c r="E51" s="41">
+        <v>500</v>
+      </c>
+      <c r="F51" s="42">
+        <v>50</v>
+      </c>
+      <c r="G51" s="42"/>
+      <c r="H51" s="42"/>
+      <c r="I51" s="42"/>
+      <c r="J51" s="42">
+        <v>43</v>
+      </c>
+      <c r="K51" s="41" t="s">
+        <v>159</v>
+      </c>
+      <c r="L51" s="41">
+        <v>14.19996213502</v>
+      </c>
+      <c r="M51" s="41">
+        <v>280.41353046697998</v>
+      </c>
+      <c r="N51" s="41">
+        <v>0.33345712373000003</v>
+      </c>
+      <c r="O51" s="41">
+        <v>0.1077331925174</v>
+      </c>
+      <c r="P51" s="41">
+        <v>5.7041712299999998E-2</v>
+      </c>
+      <c r="Q51" s="41" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="52" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A52" s="67" t="s">
+        <v>16</v>
+      </c>
+      <c r="B52" s="67">
+        <v>414</v>
+      </c>
+      <c r="C52" s="66" t="s">
+        <v>8</v>
+      </c>
+      <c r="D52" s="66"/>
+      <c r="E52" s="41">
+        <v>500</v>
+      </c>
+      <c r="F52" s="66">
+        <v>50</v>
+      </c>
+      <c r="G52" s="66"/>
+      <c r="H52" s="66"/>
+      <c r="I52" s="66"/>
+      <c r="J52" s="66">
+        <v>44</v>
+      </c>
+      <c r="K52" s="41" t="s">
+        <v>161</v>
+      </c>
+      <c r="L52" s="41">
+        <v>16.1286886983</v>
+      </c>
+      <c r="M52" s="41">
+        <v>353.53304974000002</v>
+      </c>
+      <c r="N52" s="41">
+        <v>0.3554392636</v>
+      </c>
+      <c r="O52" s="41">
+        <v>0.14522530114000001</v>
+      </c>
+      <c r="P52" s="41">
+        <v>5.1319925129999999E-2</v>
+      </c>
+      <c r="Q52" s="41" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="53" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A53" s="67"/>
+      <c r="B53" s="67"/>
+      <c r="C53" s="66"/>
+      <c r="D53" s="66"/>
+      <c r="E53" s="41"/>
+      <c r="F53" s="66"/>
+      <c r="G53" s="66"/>
+      <c r="H53" s="66"/>
+      <c r="I53" s="66"/>
+      <c r="J53" s="66"/>
+      <c r="K53" s="41"/>
+      <c r="L53" s="41"/>
+      <c r="M53" s="41"/>
+      <c r="N53" s="41"/>
+      <c r="O53" s="41"/>
+      <c r="P53" s="41"/>
+      <c r="Q53" s="41"/>
+    </row>
+    <row r="54" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A54" s="67" t="s">
+        <v>16</v>
+      </c>
+      <c r="B54" s="41">
+        <v>414</v>
+      </c>
+      <c r="C54" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="D54" s="42">
+        <v>37016</v>
+      </c>
+      <c r="E54" s="41">
+        <v>100</v>
+      </c>
+      <c r="F54" s="42">
+        <v>50</v>
+      </c>
+      <c r="G54" s="42"/>
+      <c r="H54" s="42"/>
+      <c r="I54" s="42" t="s">
+        <v>164</v>
+      </c>
+      <c r="J54" s="42">
+        <v>42</v>
+      </c>
+      <c r="K54" s="41" t="s">
+        <v>163</v>
+      </c>
+      <c r="L54" s="41">
+        <v>15.980332505</v>
+      </c>
+      <c r="M54" s="41">
+        <v>302.94736621959999</v>
+      </c>
+      <c r="N54" s="41">
+        <v>0.40205704435930001</v>
+      </c>
+      <c r="O54" s="41">
+        <v>0.31907052959999999</v>
+      </c>
+      <c r="P54" s="41">
+        <v>0.54858797000000004</v>
+      </c>
+      <c r="Q54" s="41" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="55" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A55" s="67" t="s">
+        <v>16</v>
+      </c>
+      <c r="B55" s="41">
+        <v>414</v>
+      </c>
+      <c r="C55" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="D55" s="42">
+        <v>37016</v>
+      </c>
+      <c r="E55" s="41">
+        <v>150</v>
+      </c>
+      <c r="F55" s="42">
+        <v>50</v>
+      </c>
+      <c r="G55" s="42"/>
+      <c r="H55" s="42"/>
+      <c r="I55" s="42" t="s">
+        <v>164</v>
+      </c>
+      <c r="J55" s="42">
+        <v>42</v>
+      </c>
+      <c r="K55" s="41" t="s">
+        <v>167</v>
+      </c>
+      <c r="L55" s="41">
+        <v>16.218306434750001</v>
+      </c>
+      <c r="M55" s="41">
+        <v>339.22807427999999</v>
+      </c>
+      <c r="N55" s="41">
+        <v>0.36811413275179999</v>
+      </c>
+      <c r="O55" s="41">
+        <v>0.202724971</v>
+      </c>
+      <c r="P55" s="41">
+        <v>9.3437584000000004E-2</v>
+      </c>
+      <c r="Q55" s="41" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="56" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A56" s="67" t="s">
+        <v>16</v>
+      </c>
+      <c r="B56" s="41">
+        <v>414</v>
+      </c>
+      <c r="C56" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="D56" s="42">
+        <v>37016</v>
+      </c>
+      <c r="E56" s="41">
+        <v>200</v>
+      </c>
+      <c r="F56" s="42">
+        <v>50</v>
+      </c>
+      <c r="G56" s="42"/>
+      <c r="H56" s="42"/>
+      <c r="I56" s="42" t="s">
+        <v>164</v>
+      </c>
+      <c r="J56" s="42">
+        <v>42</v>
+      </c>
+      <c r="K56" s="41" t="s">
+        <v>169</v>
+      </c>
+      <c r="L56" s="41">
+        <v>15.002265231786</v>
+      </c>
+      <c r="M56" s="41">
+        <v>308.29770306929998</v>
+      </c>
+      <c r="N56" s="41">
+        <v>0.36335503260000002</v>
+      </c>
+      <c r="O56" s="41">
+        <v>0.16385071234000001</v>
+      </c>
+      <c r="P56" s="41">
+        <v>0.21228941600000001</v>
+      </c>
+      <c r="Q56" s="41" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="57" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A57" s="67" t="s">
+        <v>16</v>
+      </c>
+      <c r="B57" s="41">
+        <v>414</v>
+      </c>
+      <c r="C57" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="D57" s="42">
+        <v>37016</v>
+      </c>
+      <c r="E57" s="41">
+        <v>250</v>
+      </c>
+      <c r="F57" s="42">
+        <v>50</v>
+      </c>
+      <c r="G57" s="42"/>
+      <c r="H57" s="42"/>
+      <c r="I57" s="42" t="s">
+        <v>164</v>
+      </c>
+      <c r="J57" s="42">
+        <v>42</v>
+      </c>
+      <c r="K57" s="41" t="s">
+        <v>171</v>
+      </c>
+      <c r="L57" s="41">
+        <v>16.282205761189999</v>
+      </c>
+      <c r="M57" s="41">
+        <v>333.53385159999999</v>
+      </c>
+      <c r="N57" s="41">
+        <v>0.36693963899999998</v>
+      </c>
+      <c r="O57" s="41">
+        <v>0.21190996557</v>
+      </c>
+      <c r="P57" s="41">
+        <v>6.8634601500000003E-2</v>
+      </c>
+      <c r="Q57" s="41" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="58" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A58" s="67" t="s">
+        <v>16</v>
+      </c>
+      <c r="B58" s="41">
+        <v>414</v>
+      </c>
+      <c r="C58" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="D58" s="42">
+        <v>37016</v>
+      </c>
+      <c r="E58" s="41">
+        <v>300</v>
+      </c>
+      <c r="F58" s="42">
+        <v>50</v>
+      </c>
+      <c r="G58" s="42"/>
+      <c r="H58" s="42"/>
+      <c r="I58" s="42" t="s">
+        <v>164</v>
+      </c>
+      <c r="J58" s="42">
+        <v>42</v>
+      </c>
+      <c r="K58" s="41" t="s">
+        <v>172</v>
+      </c>
+      <c r="L58" s="41">
+        <v>18.886168000000001</v>
+      </c>
+      <c r="M58" s="41">
+        <v>419.92427500000002</v>
+      </c>
+      <c r="N58" s="41">
+        <v>0.39891390999999998</v>
+      </c>
+      <c r="O58" s="41">
+        <v>0.28305669</v>
+      </c>
+      <c r="P58" s="41">
+        <v>7.2857166599999995E-2</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -2410,47 +3460,66 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08AF3A36-8329-4641-8F20-69FE4A8D253B}">
-  <dimension ref="A1:P33"/>
+  <dimension ref="A1:P39"/>
   <sheetViews>
     <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="7" max="7" width="13.54296875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="10.90625" style="1"/>
+    <col min="10" max="10" width="10.90625" style="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B1" s="2">
-        <v>4227</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" s="3"/>
-      <c r="E1" s="2">
-        <v>50</v>
-      </c>
-      <c r="F1" s="3">
-        <v>50</v>
-      </c>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="14">
-        <v>5.3913402057172197</v>
-      </c>
-      <c r="L1" s="15">
-        <v>95.558690835703899</v>
-      </c>
-      <c r="M1" s="15">
-        <v>4.5453329399599597E-2</v>
-      </c>
-      <c r="N1" s="15"/>
-      <c r="O1" s="15"/>
-      <c r="P1" s="3"/>
+    <row r="1" spans="1:16" s="10" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="J1" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="K1" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="L1" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="M1" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="N1" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="O1" s="11" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="2" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
@@ -2467,20 +3536,20 @@
         <v>50</v>
       </c>
       <c r="F2" s="3">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
       <c r="K2" s="14">
-        <v>4.1829039523568197</v>
+        <v>5.3913402057172197</v>
       </c>
       <c r="L2" s="15">
-        <v>45.512803344470299</v>
+        <v>95.558690835703899</v>
       </c>
       <c r="M2" s="15">
-        <v>3.7512549576846597E-2</v>
+        <v>4.5453329399599597E-2</v>
       </c>
       <c r="N2" s="15"/>
       <c r="O2" s="15"/>
@@ -2498,25 +3567,23 @@
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="2">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="F3" s="3">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
-      <c r="I3" s="3">
-        <v>42</v>
-      </c>
+      <c r="I3" s="3"/>
       <c r="J3" s="3"/>
       <c r="K3" s="14">
-        <v>3.53453446581329</v>
+        <v>4.1829039523568197</v>
       </c>
       <c r="L3" s="15">
-        <v>39.950803257038203</v>
+        <v>45.512803344470299</v>
       </c>
       <c r="M3" s="15">
-        <v>3.3774608183609799E-2</v>
+        <v>3.7512549576846597E-2</v>
       </c>
       <c r="N3" s="15"/>
       <c r="O3" s="15"/>
@@ -2541,16 +3608,18 @@
       </c>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
+      <c r="I4" s="3">
+        <v>42</v>
+      </c>
       <c r="J4" s="3"/>
       <c r="K4" s="14">
-        <v>4.3992172136277903</v>
+        <v>3.53453446581329</v>
       </c>
       <c r="L4" s="15">
-        <v>59.648501471104701</v>
+        <v>39.950803257038203</v>
       </c>
       <c r="M4" s="15">
-        <v>3.96223073497197E-2</v>
+        <v>3.3774608183609799E-2</v>
       </c>
       <c r="N4" s="15"/>
       <c r="O4" s="15"/>
@@ -2573,31 +3642,21 @@
       <c r="F5" s="3">
         <v>50</v>
       </c>
-      <c r="G5" s="3">
-        <v>14</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="I5" s="3">
-        <v>42</v>
-      </c>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
       <c r="J5" s="3"/>
       <c r="K5" s="14">
-        <v>4.9019094580076903</v>
+        <v>4.3992172136277903</v>
       </c>
       <c r="L5" s="15">
-        <v>69.704341403514405</v>
+        <v>59.648501471104701</v>
       </c>
       <c r="M5" s="15">
-        <v>4.4429586679793499E-2</v>
-      </c>
-      <c r="N5" s="15">
-        <v>4.0116878914842703E-2</v>
-      </c>
-      <c r="O5" s="15">
-        <v>2.2393254599391101E-2</v>
-      </c>
+        <v>3.96223073497197E-2</v>
+      </c>
+      <c r="N5" s="15"/>
+      <c r="O5" s="15"/>
       <c r="P5" s="3"/>
     </row>
     <row r="6" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -2624,23 +3683,23 @@
         <v>41</v>
       </c>
       <c r="I6" s="3">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J6" s="3"/>
       <c r="K6" s="14">
-        <v>4.0038073852598499</v>
+        <v>4.9019094580076903</v>
       </c>
       <c r="L6" s="15">
-        <v>53.093623329446302</v>
+        <v>69.704341403514405</v>
       </c>
       <c r="M6" s="15">
-        <v>3.6688789757854501E-2</v>
+        <v>4.4429586679793499E-2</v>
       </c>
       <c r="N6" s="15">
-        <v>3.0750500964385599E-2</v>
+        <v>4.0116878914842703E-2</v>
       </c>
       <c r="O6" s="15">
-        <v>1.4080862918083499E-2</v>
+        <v>2.2393254599391101E-2</v>
       </c>
       <c r="P6" s="3"/>
     </row>
@@ -2668,71 +3727,69 @@
         <v>41</v>
       </c>
       <c r="I7" s="3">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J7" s="3"/>
       <c r="K7" s="14">
+        <v>4.0038073852598499</v>
+      </c>
+      <c r="L7" s="15">
+        <v>53.093623329446302</v>
+      </c>
+      <c r="M7" s="15">
+        <v>3.6688789757854501E-2</v>
+      </c>
+      <c r="N7" s="15">
+        <v>3.0750500964385599E-2</v>
+      </c>
+      <c r="O7" s="15">
+        <v>1.4080862918083499E-2</v>
+      </c>
+      <c r="P7" s="3"/>
+    </row>
+    <row r="8" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="2">
+        <v>4227</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="3"/>
+      <c r="E8" s="2">
+        <v>100</v>
+      </c>
+      <c r="F8" s="3">
+        <v>50</v>
+      </c>
+      <c r="G8" s="3">
+        <v>14</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="I8" s="3">
+        <v>44</v>
+      </c>
+      <c r="J8" s="3"/>
+      <c r="K8" s="14">
         <v>3.5157139455596198</v>
       </c>
-      <c r="L7" s="15">
+      <c r="L8" s="15">
         <v>49.999309540454</v>
       </c>
-      <c r="M7" s="15">
+      <c r="M8" s="15">
         <v>3.34109955349556E-2</v>
       </c>
-      <c r="N7" s="15">
+      <c r="N8" s="15">
         <v>2.99456884654348E-2</v>
       </c>
-      <c r="O7" s="15">
+      <c r="O8" s="15">
         <v>1.5938158334067899E-2</v>
       </c>
-      <c r="P7" s="3"/>
-    </row>
-    <row r="8" spans="1:16" s="48" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="48" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" s="48">
-        <v>4227</v>
-      </c>
-      <c r="C8" s="49" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" s="49"/>
-      <c r="E8" s="48">
-        <v>100</v>
-      </c>
-      <c r="F8" s="49">
-        <v>50</v>
-      </c>
-      <c r="G8" s="49" t="s">
-        <v>57</v>
-      </c>
-      <c r="H8" s="49" t="s">
-        <v>41</v>
-      </c>
-      <c r="I8" s="49">
-        <v>42</v>
-      </c>
-      <c r="J8" s="49">
-        <v>5.4063999999999997</v>
-      </c>
-      <c r="K8" s="50">
-        <v>4.1674490000000004</v>
-      </c>
-      <c r="L8" s="51">
-        <v>59.873821397952298</v>
-      </c>
-      <c r="M8" s="51">
-        <v>3.8940099999999998E-2</v>
-      </c>
-      <c r="N8" s="51">
-        <v>3.6601000000000002E-2</v>
-      </c>
-      <c r="O8" s="51">
-        <v>2.0503E-2</v>
-      </c>
-      <c r="P8" s="49"/>
+      <c r="P8" s="3"/>
     </row>
     <row r="9" spans="1:16" s="48" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="48" t="s">
@@ -2758,25 +3815,25 @@
         <v>41</v>
       </c>
       <c r="I9" s="49">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J9" s="49">
-        <v>5.5023</v>
+        <v>5.4063999999999997</v>
       </c>
       <c r="K9" s="50">
-        <v>3.5784159999999998</v>
+        <v>4.1674490000000004</v>
       </c>
       <c r="L9" s="51">
-        <v>51.550781989999997</v>
+        <v>59.873821397952298</v>
       </c>
       <c r="M9" s="51">
-        <v>3.3480000000000003E-2</v>
+        <v>3.8940099999999998E-2</v>
       </c>
       <c r="N9" s="51">
-        <v>3.0080800000000001E-2</v>
+        <v>3.6601000000000002E-2</v>
       </c>
       <c r="O9" s="51">
-        <v>1.5723500000000001E-2</v>
+        <v>2.0503E-2</v>
       </c>
       <c r="P9" s="49"/>
     </row>
@@ -2804,25 +3861,25 @@
         <v>41</v>
       </c>
       <c r="I10" s="49">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J10" s="49">
-        <v>5.4516999999999998</v>
+        <v>5.5023</v>
       </c>
       <c r="K10" s="50">
-        <v>3.7627000000000002</v>
+        <v>3.5784159999999998</v>
       </c>
       <c r="L10" s="51">
-        <v>57.009099999999997</v>
+        <v>51.550781989999997</v>
       </c>
       <c r="M10" s="51">
-        <v>3.4901000000000001E-2</v>
+        <v>3.3480000000000003E-2</v>
       </c>
       <c r="N10" s="51">
-        <v>3.1515000000000001E-2</v>
+        <v>3.0080800000000001E-2</v>
       </c>
       <c r="O10" s="51">
-        <v>1.6348600000000001E-2</v>
+        <v>1.5723500000000001E-2</v>
       </c>
       <c r="P10" s="49"/>
     </row>
@@ -2841,7 +3898,7 @@
         <v>100</v>
       </c>
       <c r="F11" s="49">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="G11" s="49" t="s">
         <v>57</v>
@@ -2850,25 +3907,25 @@
         <v>41</v>
       </c>
       <c r="I11" s="49">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="J11" s="49">
-        <v>5.4119000000000002</v>
+        <v>5.4516999999999998</v>
       </c>
       <c r="K11" s="50">
-        <v>3.4432</v>
+        <v>3.7627000000000002</v>
       </c>
       <c r="L11" s="51">
-        <v>44.466742855213496</v>
+        <v>57.009099999999997</v>
       </c>
       <c r="M11" s="51">
-        <v>3.3230000000000003E-2</v>
+        <v>3.4901000000000001E-2</v>
       </c>
       <c r="N11" s="51">
-        <v>2.8675699999999998E-2</v>
+        <v>3.1515000000000001E-2</v>
       </c>
       <c r="O11" s="51">
-        <v>1.43138E-2</v>
+        <v>1.6348600000000001E-2</v>
       </c>
       <c r="P11" s="49"/>
     </row>
@@ -2896,25 +3953,25 @@
         <v>41</v>
       </c>
       <c r="I12" s="49">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J12" s="49">
-        <v>5.3997000000000002</v>
+        <v>5.4119000000000002</v>
       </c>
       <c r="K12" s="50">
-        <v>3.5510999999999999</v>
+        <v>3.4432</v>
       </c>
       <c r="L12" s="51">
-        <v>42.423400000000001</v>
+        <v>44.466742855213496</v>
       </c>
       <c r="M12" s="51">
-        <v>3.3779999999999998E-2</v>
+        <v>3.3230000000000003E-2</v>
       </c>
       <c r="N12" s="51">
-        <v>2.84336E-2</v>
+        <v>2.8675699999999998E-2</v>
       </c>
       <c r="O12" s="51">
-        <v>0.13858000000000001</v>
+        <v>1.43138E-2</v>
       </c>
       <c r="P12" s="49"/>
     </row>
@@ -2942,25 +3999,25 @@
         <v>41</v>
       </c>
       <c r="I13" s="49">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J13" s="49">
-        <v>5.3997999999999999</v>
+        <v>5.3997000000000002</v>
       </c>
       <c r="K13" s="50">
-        <v>3.6132961283458198</v>
+        <v>3.5510999999999999</v>
       </c>
       <c r="L13" s="51">
-        <v>42.991917761875698</v>
+        <v>42.423400000000001</v>
       </c>
       <c r="M13" s="51">
-        <v>3.40602294154084E-2</v>
+        <v>3.3779999999999998E-2</v>
       </c>
       <c r="N13" s="51">
-        <v>2.9851293000000001E-2</v>
+        <v>2.84336E-2</v>
       </c>
       <c r="O13" s="51">
-        <v>1.3512874797E-2</v>
+        <v>0.13858000000000001</v>
       </c>
       <c r="P13" s="49"/>
     </row>
@@ -2979,7 +4036,7 @@
         <v>100</v>
       </c>
       <c r="F14" s="49">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="G14" s="49" t="s">
         <v>57</v>
@@ -2988,25 +4045,25 @@
         <v>41</v>
       </c>
       <c r="I14" s="49">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="J14" s="49">
-        <v>5.3769999999999998</v>
+        <v>5.3997999999999999</v>
       </c>
       <c r="K14" s="50">
-        <v>3.4301591109624199</v>
+        <v>3.6132961283458198</v>
       </c>
       <c r="L14" s="51">
-        <v>44.733049000000001</v>
+        <v>42.991917761875698</v>
       </c>
       <c r="M14" s="51">
-        <v>3.2132932507393602E-2</v>
+        <v>3.40602294154084E-2</v>
       </c>
       <c r="N14" s="51">
-        <v>2.8753426169999999E-2</v>
+        <v>2.9851293000000001E-2</v>
       </c>
       <c r="O14" s="51">
-        <v>1.39623572084751E-2</v>
+        <v>1.3512874797E-2</v>
       </c>
       <c r="P14" s="49"/>
     </row>
@@ -3034,25 +4091,25 @@
         <v>41</v>
       </c>
       <c r="I15" s="49">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J15" s="49">
-        <v>5.3738999999999999</v>
+        <v>5.3769999999999998</v>
       </c>
       <c r="K15" s="50">
-        <v>3.4098999999999999</v>
+        <v>3.4301591109624199</v>
       </c>
       <c r="L15" s="51">
-        <v>40.6162672186896</v>
+        <v>44.733049000000001</v>
       </c>
       <c r="M15" s="51">
-        <v>3.26955353402422E-2</v>
+        <v>3.2132932507393602E-2</v>
       </c>
       <c r="N15" s="51">
-        <v>2.9034644450000001E-2</v>
+        <v>2.8753426169999999E-2</v>
       </c>
       <c r="O15" s="51">
-        <v>1.3589085000000001E-2</v>
+        <v>1.39623572084751E-2</v>
       </c>
       <c r="P15" s="49"/>
     </row>
@@ -3080,73 +4137,73 @@
         <v>41</v>
       </c>
       <c r="I16" s="49">
+        <v>43</v>
+      </c>
+      <c r="J16" s="49">
+        <v>5.3738999999999999</v>
+      </c>
+      <c r="K16" s="50">
+        <v>3.4098999999999999</v>
+      </c>
+      <c r="L16" s="51">
+        <v>40.6162672186896</v>
+      </c>
+      <c r="M16" s="51">
+        <v>3.26955353402422E-2</v>
+      </c>
+      <c r="N16" s="51">
+        <v>2.9034644450000001E-2</v>
+      </c>
+      <c r="O16" s="51">
+        <v>1.3589085000000001E-2</v>
+      </c>
+      <c r="P16" s="49"/>
+    </row>
+    <row r="17" spans="1:16" s="48" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="48" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" s="48">
+        <v>4227</v>
+      </c>
+      <c r="C17" s="49" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" s="49"/>
+      <c r="E17" s="48">
+        <v>100</v>
+      </c>
+      <c r="F17" s="49">
+        <v>150</v>
+      </c>
+      <c r="G17" s="49" t="s">
+        <v>57</v>
+      </c>
+      <c r="H17" s="49" t="s">
+        <v>41</v>
+      </c>
+      <c r="I17" s="49">
         <v>44</v>
       </c>
-      <c r="J16" s="49">
+      <c r="J17" s="49">
         <v>5.3731999999999998</v>
       </c>
-      <c r="K16" s="50">
+      <c r="K17" s="50">
         <v>4.0764711262509703</v>
       </c>
-      <c r="L16" s="51">
+      <c r="L17" s="51">
         <v>53.140005000000002</v>
       </c>
-      <c r="M16" s="51">
+      <c r="M17" s="51">
         <v>3.8317999999999998E-2</v>
       </c>
-      <c r="N16" s="51">
+      <c r="N17" s="51">
         <v>3.4648360299304001E-2</v>
       </c>
-      <c r="O16" s="51">
+      <c r="O17" s="51">
         <v>1.7697500000000001E-2</v>
       </c>
-      <c r="P16" s="49"/>
-    </row>
-    <row r="17" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B17" s="2">
-        <v>4227</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D17" s="3"/>
-      <c r="E17" s="2">
-        <v>100</v>
-      </c>
-      <c r="F17" s="3">
-        <v>100</v>
-      </c>
-      <c r="G17" s="3">
-        <v>14</v>
-      </c>
-      <c r="H17" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="I17" s="3">
-        <v>42</v>
-      </c>
-      <c r="J17" s="3">
-        <v>5.3731</v>
-      </c>
-      <c r="K17" s="14">
-        <v>4.6888277983732802</v>
-      </c>
-      <c r="L17" s="15">
-        <v>58.546133147207897</v>
-      </c>
-      <c r="M17" s="15">
-        <v>4.2354736963695502E-2</v>
-      </c>
-      <c r="N17" s="15">
-        <v>3.81307362333883E-2</v>
-      </c>
-      <c r="O17" s="15">
-        <v>1.94263506138064E-2</v>
-      </c>
-      <c r="P17" s="3"/>
+      <c r="P17" s="49"/>
     </row>
     <row r="18" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
@@ -3172,25 +4229,25 @@
         <v>41</v>
       </c>
       <c r="I18" s="3">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J18" s="3">
-        <v>5.3796999999999997</v>
+        <v>5.3731</v>
       </c>
       <c r="K18" s="14">
-        <v>3.76198040986064</v>
+        <v>4.6888277983732802</v>
       </c>
       <c r="L18" s="15">
-        <v>42.1346287254948</v>
+        <v>58.546133147207897</v>
       </c>
       <c r="M18" s="15">
-        <v>3.5131886546129497E-2</v>
+        <v>4.2354736963695502E-2</v>
       </c>
       <c r="N18" s="15">
-        <v>3.1839711844375E-2</v>
+        <v>3.81307362333883E-2</v>
       </c>
       <c r="O18" s="15">
-        <v>1.50434441822506E-2</v>
+        <v>1.94263506138064E-2</v>
       </c>
       <c r="P18" s="3"/>
     </row>
@@ -3218,41 +4275,72 @@
         <v>41</v>
       </c>
       <c r="I19" s="3">
+        <v>43</v>
+      </c>
+      <c r="J19" s="3">
+        <v>5.3796999999999997</v>
+      </c>
+      <c r="K19" s="14">
+        <v>3.76198040986064</v>
+      </c>
+      <c r="L19" s="15">
+        <v>42.1346287254948</v>
+      </c>
+      <c r="M19" s="15">
+        <v>3.5131886546129497E-2</v>
+      </c>
+      <c r="N19" s="15">
+        <v>3.1839711844375E-2</v>
+      </c>
+      <c r="O19" s="15">
+        <v>1.50434441822506E-2</v>
+      </c>
+      <c r="P19" s="3"/>
+    </row>
+    <row r="20" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20" s="2">
+        <v>4227</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D20" s="3"/>
+      <c r="E20" s="2">
+        <v>100</v>
+      </c>
+      <c r="F20" s="3">
+        <v>100</v>
+      </c>
+      <c r="G20" s="3">
+        <v>14</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="I20" s="3">
         <v>44</v>
       </c>
-      <c r="J19" s="3">
+      <c r="J20" s="3">
         <v>5.3815999999999997</v>
       </c>
-      <c r="K19" s="14">
+      <c r="K20" s="14">
         <v>3.7490946166483901</v>
       </c>
-      <c r="L19" s="15">
+      <c r="L20" s="15">
         <v>44.046071467776798</v>
       </c>
-      <c r="M19" s="15">
+      <c r="M20" s="15">
         <v>3.4733060718235398E-2</v>
       </c>
-      <c r="N19" s="15">
+      <c r="N20" s="15">
         <v>3.1557588852523799E-2</v>
       </c>
-      <c r="O19" s="15">
+      <c r="O20" s="15">
         <v>1.4121308543102401E-2</v>
       </c>
-      <c r="P19" s="3"/>
-    </row>
-    <row r="20" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
-      <c r="I20" s="3"/>
-      <c r="J20" s="3"/>
-      <c r="K20" s="14"/>
-      <c r="L20" s="15"/>
-      <c r="M20" s="15"/>
-      <c r="N20" s="15"/>
-      <c r="O20" s="15"/>
       <c r="P20" s="3"/>
     </row>
     <row r="21" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -3271,35 +4359,16 @@
       <c r="P21" s="3"/>
     </row>
     <row r="22" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B22" s="2">
-        <v>4227</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>9</v>
-      </c>
+      <c r="C22" s="3"/>
       <c r="D22" s="3"/>
-      <c r="E22" s="2">
-        <v>100</v>
-      </c>
-      <c r="F22" s="3">
-        <v>100</v>
-      </c>
+      <c r="F22" s="3"/>
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
       <c r="I22" s="3"/>
       <c r="J22" s="3"/>
-      <c r="K22" s="14">
-        <v>3.4822369638914501</v>
-      </c>
-      <c r="L22" s="15">
-        <v>38.929181310867698</v>
-      </c>
-      <c r="M22" s="15">
-        <v>3.3039162166202E-2</v>
-      </c>
+      <c r="K22" s="14"/>
+      <c r="L22" s="15"/>
+      <c r="M22" s="15"/>
       <c r="N22" s="15"/>
       <c r="O22" s="15"/>
       <c r="P22" s="3"/>
@@ -3319,27 +4388,23 @@
         <v>100</v>
       </c>
       <c r="F23" s="3">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
       <c r="I23" s="3"/>
       <c r="J23" s="3"/>
       <c r="K23" s="14">
-        <v>3.4948489288649101</v>
+        <v>3.4822369638914501</v>
       </c>
       <c r="L23" s="15">
-        <v>39.458377616161002</v>
+        <v>38.929181310867698</v>
       </c>
       <c r="M23" s="15">
-        <v>3.3644492587488403E-2</v>
-      </c>
-      <c r="N23" s="15">
-        <v>3.00505847160191E-2</v>
-      </c>
-      <c r="O23" s="15">
-        <v>1.43563269479154E-2</v>
-      </c>
+        <v>3.3039162166202E-2</v>
+      </c>
+      <c r="N23" s="15"/>
+      <c r="O23" s="15"/>
       <c r="P23" s="3"/>
     </row>
     <row r="24" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -3357,34 +4422,26 @@
         <v>100</v>
       </c>
       <c r="F24" s="3">
-        <v>200</v>
-      </c>
-      <c r="G24" s="3">
-        <v>14</v>
-      </c>
-      <c r="H24" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="I24" s="3">
-        <v>42</v>
-      </c>
-      <c r="J24" s="3">
-        <v>5.3231000000000002</v>
-      </c>
+        <v>150</v>
+      </c>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="3"/>
+      <c r="J24" s="3"/>
       <c r="K24" s="14">
-        <v>5.40633569574379</v>
+        <v>3.4948489288649101</v>
       </c>
       <c r="L24" s="15">
-        <v>77.864039181710595</v>
+        <v>39.458377616161002</v>
       </c>
       <c r="M24" s="15">
-        <v>4.7543834963823403E-2</v>
+        <v>3.3644492587488403E-2</v>
       </c>
       <c r="N24" s="15">
-        <v>4.598874E-2</v>
+        <v>3.00505847160191E-2</v>
       </c>
       <c r="O24" s="15">
-        <v>2.6339886999999999E-2</v>
+        <v>1.43563269479154E-2</v>
       </c>
       <c r="P24" s="3"/>
     </row>
@@ -3398,7 +4455,9 @@
       <c r="C25" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D25" s="3"/>
+      <c r="D25" s="3">
+        <v>97983</v>
+      </c>
       <c r="E25" s="2">
         <v>100</v>
       </c>
@@ -3412,25 +4471,25 @@
         <v>41</v>
       </c>
       <c r="I25" s="3">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J25" s="3">
-        <v>5.3291000000000004</v>
+        <v>5.3231000000000002</v>
       </c>
       <c r="K25" s="14">
-        <v>4.3779429482645398</v>
+        <v>5.40633569574379</v>
       </c>
       <c r="L25" s="15">
-        <v>53.407499999999999</v>
+        <v>77.864039181710595</v>
       </c>
       <c r="M25" s="15">
-        <v>3.9220900000000003E-2</v>
+        <v>4.7543834963823403E-2</v>
       </c>
       <c r="N25" s="15">
-        <v>3.7683399999999999E-2</v>
+        <v>4.598874E-2</v>
       </c>
       <c r="O25" s="15">
-        <v>1.7714669999999998E-2</v>
+        <v>2.6339886999999999E-2</v>
       </c>
       <c r="P25" s="3"/>
     </row>
@@ -3444,7 +4503,9 @@
       <c r="C26" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D26" s="3"/>
+      <c r="D26" s="3">
+        <v>97983</v>
+      </c>
       <c r="E26" s="2">
         <v>100</v>
       </c>
@@ -3458,328 +4519,452 @@
         <v>41</v>
       </c>
       <c r="I26" s="3">
+        <v>43</v>
+      </c>
+      <c r="J26" s="3">
+        <v>5.3291000000000004</v>
+      </c>
+      <c r="K26" s="14">
+        <v>4.3779429482645398</v>
+      </c>
+      <c r="L26" s="15">
+        <v>53.407499999999999</v>
+      </c>
+      <c r="M26" s="15">
+        <v>3.9220900000000003E-2</v>
+      </c>
+      <c r="N26" s="15">
+        <v>3.7683399999999999E-2</v>
+      </c>
+      <c r="O26" s="15">
+        <v>1.7714669999999998E-2</v>
+      </c>
+      <c r="P26" s="3"/>
+    </row>
+    <row r="27" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B27" s="2">
+        <v>4227</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D27" s="3">
+        <v>97983</v>
+      </c>
+      <c r="E27" s="2">
+        <v>100</v>
+      </c>
+      <c r="F27" s="3">
+        <v>200</v>
+      </c>
+      <c r="G27" s="3">
+        <v>14</v>
+      </c>
+      <c r="H27" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="I27" s="3">
         <v>44</v>
       </c>
-      <c r="J26" s="3">
+      <c r="J27" s="3">
         <v>5.3293999999999997</v>
       </c>
-      <c r="K26" s="14">
+      <c r="K27" s="14">
         <v>3.6071879999999998</v>
       </c>
-      <c r="L26" s="15">
+      <c r="L27" s="15">
         <v>43.212336000000001</v>
       </c>
-      <c r="M26" s="15">
+      <c r="M27" s="15">
         <v>3.3841510612267103E-2</v>
       </c>
-      <c r="N26" s="15">
+      <c r="N27" s="15">
         <v>3.0669129E-2</v>
       </c>
-      <c r="O26" s="15">
+      <c r="O27" s="15">
         <v>1.4138269E-2</v>
       </c>
-      <c r="P26" s="3"/>
-    </row>
-    <row r="27" spans="1:16" s="37" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="37" t="s">
+      <c r="P27" s="3"/>
+    </row>
+    <row r="28" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+      <c r="I28" s="3"/>
+      <c r="J28" s="3"/>
+      <c r="K28" s="14"/>
+      <c r="L28" s="15"/>
+      <c r="M28" s="15"/>
+      <c r="N28" s="15"/>
+      <c r="O28" s="15"/>
+      <c r="P28" s="3"/>
+    </row>
+    <row r="29" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+      <c r="I29" s="3"/>
+      <c r="J29" s="3"/>
+      <c r="K29" s="14"/>
+      <c r="L29" s="15"/>
+      <c r="M29" s="15"/>
+      <c r="N29" s="15"/>
+      <c r="O29" s="15"/>
+      <c r="P29" s="3"/>
+    </row>
+    <row r="30" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="3"/>
+      <c r="I30" s="3"/>
+      <c r="J30" s="3"/>
+      <c r="K30" s="14"/>
+      <c r="L30" s="15"/>
+      <c r="M30" s="15"/>
+      <c r="N30" s="15"/>
+      <c r="O30" s="15"/>
+      <c r="P30" s="3"/>
+    </row>
+    <row r="31" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="3"/>
+      <c r="I31" s="3"/>
+      <c r="J31" s="3"/>
+      <c r="K31" s="14"/>
+      <c r="L31" s="15"/>
+      <c r="M31" s="15"/>
+      <c r="N31" s="15"/>
+      <c r="O31" s="15"/>
+      <c r="P31" s="3"/>
+    </row>
+    <row r="32" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="3"/>
+      <c r="H32" s="3"/>
+      <c r="I32" s="3"/>
+      <c r="J32" s="3"/>
+      <c r="K32" s="14"/>
+      <c r="L32" s="15"/>
+      <c r="M32" s="15"/>
+      <c r="N32" s="15"/>
+      <c r="O32" s="15"/>
+      <c r="P32" s="3"/>
+    </row>
+    <row r="33" spans="1:16" s="37" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="B27" s="37">
+      <c r="B33" s="37">
         <v>4227</v>
       </c>
-      <c r="C27" s="38" t="s">
+      <c r="C33" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="D27" s="38"/>
-      <c r="E27" s="37">
+      <c r="D33" s="38"/>
+      <c r="E33" s="37">
         <v>25</v>
       </c>
-      <c r="F27" s="38">
-        <v>50</v>
-      </c>
-      <c r="G27" s="38"/>
-      <c r="H27" s="38"/>
-      <c r="I27" s="38">
+      <c r="F33" s="38">
+        <v>50</v>
+      </c>
+      <c r="G33" s="38"/>
+      <c r="H33" s="38"/>
+      <c r="I33" s="38">
         <v>42</v>
       </c>
-      <c r="J27" s="38"/>
-      <c r="K27" s="39">
+      <c r="J33" s="38"/>
+      <c r="K33" s="39">
         <v>3.7265029427634002</v>
       </c>
-      <c r="L27" s="40">
+      <c r="L33" s="40">
         <v>45.614512805679603</v>
       </c>
-      <c r="M27" s="39">
+      <c r="M33" s="39">
         <v>3.43615135073616E-2</v>
       </c>
-      <c r="N27" s="39">
+      <c r="N33" s="39">
         <v>3.1547316617100397E-2</v>
       </c>
-      <c r="O27" s="39">
+      <c r="O33" s="39">
         <v>1.5534556490396E-2</v>
       </c>
-      <c r="P27" s="38"/>
-    </row>
-    <row r="28" spans="1:16" s="37" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="37" t="s">
+      <c r="P33" s="38"/>
+    </row>
+    <row r="34" spans="1:16" s="37" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="B28" s="37">
+      <c r="B34" s="37">
         <v>4227</v>
       </c>
-      <c r="C28" s="38" t="s">
+      <c r="C34" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="D28" s="38">
+      <c r="D34" s="38">
         <v>240609</v>
       </c>
-      <c r="E28" s="37">
+      <c r="E34" s="37">
         <v>25</v>
       </c>
-      <c r="F28" s="38">
-        <v>50</v>
-      </c>
-      <c r="G28" s="38"/>
-      <c r="H28" s="38" t="s">
+      <c r="F34" s="38">
+        <v>50</v>
+      </c>
+      <c r="G34" s="38"/>
+      <c r="H34" s="38" t="s">
         <v>41</v>
       </c>
-      <c r="I28" s="38">
+      <c r="I34" s="38">
         <v>42</v>
       </c>
-      <c r="J28" s="38">
+      <c r="J34" s="38">
         <v>-2.4544000000000001</v>
       </c>
-      <c r="K28" s="39">
+      <c r="K34" s="39">
         <v>3.8999714860000001</v>
       </c>
-      <c r="L28" s="40">
+      <c r="L34" s="40">
         <v>53.729131000000002</v>
       </c>
-      <c r="M28" s="40">
+      <c r="M34" s="40">
         <v>3.6286051999999999E-2</v>
       </c>
-      <c r="N28" s="40">
+      <c r="N34" s="40">
         <v>3.3511891500000002E-2</v>
       </c>
-      <c r="O28" s="40">
+      <c r="O34" s="40">
         <v>1.95500176E-2</v>
       </c>
-      <c r="P28" s="38"/>
-    </row>
-    <row r="29" spans="1:16" s="37" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="37" t="s">
+      <c r="P34" s="38"/>
+    </row>
+    <row r="35" spans="1:16" s="37" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="B29" s="37">
+      <c r="B35" s="37">
         <v>4227</v>
       </c>
-      <c r="C29" s="38" t="s">
+      <c r="C35" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="D29" s="38">
+      <c r="D35" s="38">
         <v>240609</v>
       </c>
-      <c r="E29" s="37">
+      <c r="E35" s="37">
         <v>25</v>
       </c>
-      <c r="F29" s="38">
-        <v>50</v>
-      </c>
-      <c r="G29" s="38"/>
-      <c r="H29" s="38" t="s">
+      <c r="F35" s="38">
+        <v>50</v>
+      </c>
+      <c r="G35" s="38"/>
+      <c r="H35" s="38" t="s">
         <v>41</v>
       </c>
-      <c r="I29" s="38">
+      <c r="I35" s="38">
         <v>43</v>
       </c>
-      <c r="J29" s="38">
+      <c r="J35" s="38">
         <v>-2.4998999999999998</v>
       </c>
-      <c r="K29" s="39">
+      <c r="K35" s="39">
         <v>3.9447550800000002</v>
       </c>
-      <c r="L29" s="40">
+      <c r="L35" s="40">
         <v>68.021673059999998</v>
       </c>
-      <c r="M29" s="40">
+      <c r="M35" s="40">
         <v>3.63133411E-2</v>
       </c>
-      <c r="N29" s="40">
+      <c r="N35" s="40">
         <v>3.3797269999999997E-2</v>
       </c>
-      <c r="O29" s="40">
+      <c r="O35" s="40">
         <v>2.2926808E-2</v>
       </c>
-      <c r="P29" s="38"/>
-    </row>
-    <row r="30" spans="1:16" s="37" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="37" t="s">
+      <c r="P35" s="38"/>
+    </row>
+    <row r="36" spans="1:16" s="37" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="B30" s="37">
+      <c r="B36" s="37">
         <v>4227</v>
       </c>
-      <c r="C30" s="38" t="s">
+      <c r="C36" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="D30" s="38">
+      <c r="D36" s="38">
         <v>240609</v>
       </c>
-      <c r="E30" s="37">
+      <c r="E36" s="37">
         <v>25</v>
       </c>
-      <c r="F30" s="38">
-        <v>50</v>
-      </c>
-      <c r="G30" s="38"/>
-      <c r="H30" s="38" t="s">
+      <c r="F36" s="38">
+        <v>50</v>
+      </c>
+      <c r="G36" s="38"/>
+      <c r="H36" s="38" t="s">
         <v>41</v>
       </c>
-      <c r="I30" s="38">
+      <c r="I36" s="38">
         <v>44</v>
       </c>
-      <c r="J30" s="38">
+      <c r="J36" s="38">
         <v>-2.5280999999999998</v>
       </c>
-      <c r="K30" s="39">
+      <c r="K36" s="39">
         <v>3.9255741059</v>
       </c>
-      <c r="L30" s="40">
+      <c r="L36" s="40">
         <v>67.52120601</v>
       </c>
-      <c r="M30" s="40">
+      <c r="M36" s="40">
         <v>3.6533299999999998E-2</v>
       </c>
-      <c r="N30" s="40">
+      <c r="N36" s="40">
         <v>3.3730811200000002E-2</v>
       </c>
-      <c r="O30" s="40">
+      <c r="O36" s="40">
         <v>2.29461405E-2</v>
       </c>
-      <c r="P30" s="38"/>
-    </row>
-    <row r="31" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="6" t="s">
+      <c r="P36" s="38"/>
+    </row>
+    <row r="37" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B31" s="6">
+      <c r="B37" s="6">
         <v>4227</v>
       </c>
-      <c r="C31" s="7" t="s">
+      <c r="C37" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D31" s="7"/>
-      <c r="E31" s="6">
-        <v>100</v>
-      </c>
-      <c r="F31" s="7">
-        <v>50</v>
-      </c>
-      <c r="G31" s="7"/>
-      <c r="H31" s="7"/>
-      <c r="I31" s="7">
+      <c r="D37" s="7"/>
+      <c r="E37" s="6">
+        <v>100</v>
+      </c>
+      <c r="F37" s="7">
+        <v>50</v>
+      </c>
+      <c r="G37" s="7"/>
+      <c r="H37" s="7"/>
+      <c r="I37" s="7">
         <v>42</v>
       </c>
-      <c r="J31" s="7"/>
-      <c r="K31" s="20">
+      <c r="J37" s="7"/>
+      <c r="K37" s="20">
         <v>39.8111117321926</v>
       </c>
-      <c r="L31" s="21">
+      <c r="L37" s="21">
         <v>1532.6129417120101</v>
       </c>
-      <c r="M31" s="21">
+      <c r="M37" s="21">
         <v>0.295085285407581</v>
       </c>
-      <c r="N31" s="21">
+      <c r="N37" s="21">
         <v>0.305712224216657</v>
       </c>
-      <c r="O31" s="21">
+      <c r="O37" s="21">
         <v>0.28655775903000102</v>
       </c>
-      <c r="P31" s="7"/>
-    </row>
-    <row r="32" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="6" t="s">
+      <c r="P37" s="7"/>
+    </row>
+    <row r="38" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B32" s="6">
+      <c r="B38" s="6">
         <v>4227</v>
       </c>
-      <c r="C32" s="7" t="s">
+      <c r="C38" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D32" s="7"/>
-      <c r="E32" s="6">
-        <v>100</v>
-      </c>
-      <c r="F32" s="7">
-        <v>100</v>
-      </c>
-      <c r="G32" s="7"/>
-      <c r="H32" s="7"/>
-      <c r="I32" s="7">
+      <c r="D38" s="7"/>
+      <c r="E38" s="6">
+        <v>100</v>
+      </c>
+      <c r="F38" s="7">
+        <v>100</v>
+      </c>
+      <c r="G38" s="7"/>
+      <c r="H38" s="7"/>
+      <c r="I38" s="7">
         <v>42</v>
       </c>
-      <c r="J32" s="7"/>
-      <c r="K32" s="20">
+      <c r="J38" s="7"/>
+      <c r="K38" s="20">
         <v>24.7464336651162</v>
       </c>
-      <c r="L32" s="21">
+      <c r="L38" s="21">
         <v>881.43752107056503</v>
       </c>
-      <c r="M32" s="20">
+      <c r="M38" s="20">
         <v>0.19131980000000001</v>
       </c>
-      <c r="N32" s="20">
+      <c r="N38" s="20">
         <v>0.19190260000000001</v>
       </c>
-      <c r="O32" s="21"/>
-      <c r="P32" s="7"/>
-    </row>
-    <row r="33" spans="1:16" s="25" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="25" t="s">
+      <c r="O38" s="21"/>
+      <c r="P38" s="7"/>
+    </row>
+    <row r="39" spans="1:16" s="25" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="B33" s="25">
+      <c r="B39" s="25">
         <v>4227</v>
       </c>
-      <c r="C33" s="26" t="s">
+      <c r="C39" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="D33" s="26"/>
-      <c r="E33" s="25">
-        <v>100</v>
-      </c>
-      <c r="F33" s="26">
+      <c r="D39" s="26"/>
+      <c r="E39" s="25">
+        <v>100</v>
+      </c>
+      <c r="F39" s="26">
         <v>200</v>
       </c>
-      <c r="G33" s="26"/>
-      <c r="H33" s="26"/>
-      <c r="I33" s="26">
+      <c r="G39" s="26"/>
+      <c r="H39" s="26"/>
+      <c r="I39" s="26">
         <v>42</v>
       </c>
-      <c r="J33" s="26"/>
-      <c r="K33" s="26" t="s">
+      <c r="J39" s="26"/>
+      <c r="K39" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="L33" s="25" t="s">
+      <c r="L39" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="M33" s="26" t="s">
+      <c r="M39" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="N33" s="26" t="s">
+      <c r="N39" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="O33" s="26" t="s">
+      <c r="O39" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="P33" s="26" t="s">
+      <c r="P39" s="26" t="s">
         <v>24</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>